<commit_message>
Alterações no script + Relatório .rmd
</commit_message>
<xml_diff>
--- a/dados/relatorio_historico.xlsx
+++ b/dados/relatorio_historico.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\arian\Desktop\R_STF\Relatorio_R\dados\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\arian\Desktop\R_STF\Relatorio_R\Git\Code-Relatorio\dados\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7FE6EA6-70D2-4032-92F7-C9D222200CE6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEB73A79-5996-422B-9D4C-C8FC0D4712ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11160" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11160" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="acervo" sheetId="1" r:id="rId1"/>
@@ -711,7 +711,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="71">
+  <cellXfs count="72">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -899,6 +899,7 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="3" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3413,10 +3414,10 @@
   <sheetPr>
     <tabColor rgb="FF00B050"/>
   </sheetPr>
-  <dimension ref="A1:Q16"/>
+  <dimension ref="A1:Q19"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="J18" sqref="J18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3494,7 +3495,7 @@
         <v>90331</v>
       </c>
       <c r="C2" s="39">
-        <v>12913</v>
+        <v>12907</v>
       </c>
       <c r="D2" s="39">
         <v>77418</v>
@@ -3553,7 +3554,7 @@
         <v>103650</v>
       </c>
       <c r="C3" s="39">
-        <v>28632</v>
+        <v>18632</v>
       </c>
       <c r="D3" s="39">
         <v>75018</v>
@@ -3612,7 +3613,7 @@
         <v>101947</v>
       </c>
       <c r="C4" s="39">
-        <v>21200</v>
+        <v>20750</v>
       </c>
       <c r="D4" s="39">
         <v>80747</v>
@@ -3671,7 +3672,7 @@
         <v>93197</v>
       </c>
       <c r="C5" s="39">
-        <v>21481</v>
+        <v>21301</v>
       </c>
       <c r="D5" s="39">
         <v>71716</v>
@@ -3810,6 +3811,11 @@
       <c r="P12" s="16"/>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="C13" s="71"/>
+      <c r="D13" s="71"/>
+      <c r="E13" s="71"/>
+      <c r="F13" s="71"/>
+      <c r="G13" s="71"/>
       <c r="J13" s="14"/>
       <c r="P13" s="13"/>
     </row>
@@ -3819,11 +3825,22 @@
       <c r="Q14" s="4"/>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="C15" s="71"/>
       <c r="J15" s="14"/>
       <c r="P15" s="15"/>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="C16" s="71"/>
       <c r="P16" s="15"/>
+    </row>
+    <row r="17" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C17" s="71"/>
+    </row>
+    <row r="18" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C18" s="71"/>
+    </row>
+    <row r="19" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C19" s="71"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4454,7 +4471,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{81CF680A-4DE0-4B0B-AF6A-8D59BB1A8E7B}">
   <dimension ref="A1:H22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Alterações realizadas no relatório até 06/12/2021.
</commit_message>
<xml_diff>
--- a/dados/relatorio_historico.xlsx
+++ b/dados/relatorio_historico.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\arian\Desktop\R_STF\Relatorio_R\Git\Code-Relatorio\dados\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83DE6463-BD2F-45B0-8F83-CDA7369B94F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{349B585B-AAD3-430E-90CD-BCAEC1E7D775}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11160" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11160" firstSheet="1" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="acervo" sheetId="1" r:id="rId1"/>
@@ -146,7 +146,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="289" uniqueCount="103">
   <si>
     <t>ano</t>
   </si>
@@ -459,9 +459,6 @@
   </si>
   <si>
     <t>STA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  </t>
   </si>
 </sst>
 </file>
@@ -471,7 +468,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0%"/>
   </numFmts>
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -493,11 +490,6 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
     </font>
@@ -507,12 +499,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
@@ -714,7 +700,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="72">
+  <cellXfs count="65">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -725,10 +711,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment readingOrder="1"/>
     </xf>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="10" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="10" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment readingOrder="1"/>
     </xf>
@@ -744,35 +729,27 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="9" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -781,16 +758,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="3" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="1" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment readingOrder="1"/>
     </xf>
@@ -803,22 +779,22 @@
     <xf numFmtId="1" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
@@ -830,10 +806,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
@@ -860,34 +836,34 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="9" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="9" fontId="7" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="5" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -902,7 +878,6 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="3" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1392,24 +1367,24 @@
       <c r="A6" s="1">
         <v>2020</v>
       </c>
-      <c r="B6" s="18">
+      <c r="B6" s="13">
         <v>13197</v>
       </c>
-      <c r="C6" s="18">
+      <c r="C6" s="13">
         <v>13059</v>
       </c>
-      <c r="D6" s="17">
+      <c r="D6" s="12">
         <f>1-E6</f>
         <v>0.96</v>
       </c>
-      <c r="E6" s="17">
+      <c r="E6" s="12">
         <v>0.04</v>
       </c>
-      <c r="F6" s="18">
+      <c r="F6" s="13">
         <f t="shared" si="0"/>
         <v>26256</v>
       </c>
-      <c r="G6" s="19"/>
+      <c r="G6" s="14"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1434,25 +1409,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="C1" s="10" t="s">
+      <c r="C1" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="D1" s="10" t="s">
+      <c r="D1" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="E1" s="10" t="s">
+      <c r="E1" s="9" t="s">
         <v>56</v>
       </c>
-      <c r="F1" s="11" t="s">
+      <c r="F1" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="G1" s="8" t="s">
+      <c r="G1" s="7" t="s">
         <v>58</v>
       </c>
     </row>
@@ -1463,19 +1438,19 @@
       <c r="B2" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="C2" s="32">
+      <c r="C2" s="26">
         <v>6</v>
       </c>
-      <c r="D2" s="32">
+      <c r="D2" s="26">
         <v>6</v>
       </c>
-      <c r="E2" s="32">
+      <c r="E2" s="26">
         <v>8</v>
       </c>
-      <c r="F2" s="33">
+      <c r="F2" s="27">
         <v>7</v>
       </c>
-      <c r="G2" s="34">
+      <c r="G2" s="28">
         <v>8</v>
       </c>
     </row>
@@ -1486,19 +1461,19 @@
       <c r="B3" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="C3" s="32">
+      <c r="C3" s="26">
         <v>195</v>
       </c>
-      <c r="D3" s="32">
+      <c r="D3" s="26">
         <v>237</v>
       </c>
-      <c r="E3" s="32">
+      <c r="E3" s="26">
         <v>178</v>
       </c>
-      <c r="F3" s="33">
+      <c r="F3" s="27">
         <v>241</v>
       </c>
-      <c r="G3" s="34">
+      <c r="G3" s="28">
         <v>354</v>
       </c>
     </row>
@@ -1509,19 +1484,19 @@
       <c r="B4" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="C4" s="32">
+      <c r="C4" s="26">
         <v>1</v>
       </c>
-      <c r="D4" s="32">
+      <c r="D4" s="26">
         <v>9</v>
       </c>
-      <c r="E4" s="32">
+      <c r="E4" s="26">
         <v>5</v>
       </c>
-      <c r="F4" s="33">
+      <c r="F4" s="27">
         <v>4</v>
       </c>
-      <c r="G4" s="34">
+      <c r="G4" s="28">
         <v>6</v>
       </c>
     </row>
@@ -1532,65 +1507,65 @@
       <c r="B5" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="C5" s="32">
+      <c r="C5" s="26">
         <v>60</v>
       </c>
-      <c r="D5" s="32">
+      <c r="D5" s="26">
         <v>68</v>
       </c>
-      <c r="E5" s="32">
+      <c r="E5" s="26">
         <v>54</v>
       </c>
-      <c r="F5" s="33">
+      <c r="F5" s="27">
         <v>82</v>
       </c>
-      <c r="G5" s="34">
+      <c r="G5" s="28">
         <v>135</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="53" t="s">
+      <c r="A6" s="47" t="s">
         <v>101</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="C6" s="32">
+      <c r="C6" s="26">
         <v>27</v>
       </c>
-      <c r="D6" s="32">
+      <c r="D6" s="26">
         <v>25</v>
       </c>
-      <c r="E6" s="32">
+      <c r="E6" s="26">
         <v>12</v>
       </c>
-      <c r="F6" s="33">
+      <c r="F6" s="27">
         <v>6</v>
       </c>
-      <c r="G6" s="34">
+      <c r="G6" s="28">
         <v>2</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="53" t="s">
+      <c r="A7" s="47" t="s">
         <v>100</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="C7" s="32">
+      <c r="C7" s="26">
         <v>1</v>
       </c>
-      <c r="D7" s="32">
-        <v>0</v>
-      </c>
-      <c r="E7" s="32">
-        <v>0</v>
-      </c>
-      <c r="F7" s="33">
+      <c r="D7" s="26">
+        <v>0</v>
+      </c>
+      <c r="E7" s="26">
+        <v>0</v>
+      </c>
+      <c r="F7" s="27">
         <v>1</v>
       </c>
-      <c r="G7" s="34">
+      <c r="G7" s="28">
         <v>3</v>
       </c>
     </row>
@@ -1601,19 +1576,19 @@
       <c r="B8" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="C8" s="32">
+      <c r="C8" s="26">
         <v>48</v>
       </c>
-      <c r="D8" s="32">
+      <c r="D8" s="26">
         <v>33</v>
       </c>
-      <c r="E8" s="32">
+      <c r="E8" s="26">
         <v>34</v>
       </c>
-      <c r="F8" s="33">
+      <c r="F8" s="27">
         <v>38</v>
       </c>
-      <c r="G8" s="34">
+      <c r="G8" s="28">
         <v>22</v>
       </c>
     </row>
@@ -1624,19 +1599,19 @@
       <c r="B9" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="C9" s="32">
+      <c r="C9" s="26">
         <v>6554</v>
       </c>
-      <c r="D9" s="32">
+      <c r="D9" s="26">
         <v>11327</v>
       </c>
-      <c r="E9" s="32">
+      <c r="E9" s="26">
         <v>13815</v>
       </c>
-      <c r="F9" s="33">
+      <c r="F9" s="27">
         <v>11784</v>
       </c>
-      <c r="G9" s="34">
+      <c r="G9" s="28">
         <v>14295</v>
       </c>
     </row>
@@ -1647,19 +1622,19 @@
       <c r="B10" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="C10" s="32">
+      <c r="C10" s="26">
         <v>136</v>
       </c>
-      <c r="D10" s="32">
+      <c r="D10" s="26">
         <v>233</v>
       </c>
-      <c r="E10" s="32">
+      <c r="E10" s="26">
         <v>43</v>
       </c>
-      <c r="F10" s="33">
+      <c r="F10" s="27">
         <v>15</v>
       </c>
-      <c r="G10" s="34">
+      <c r="G10" s="28">
         <v>13</v>
       </c>
     </row>
@@ -1670,19 +1645,19 @@
       <c r="B11" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="C11" s="32">
+      <c r="C11" s="26">
         <v>34</v>
       </c>
-      <c r="D11" s="32">
+      <c r="D11" s="26">
         <v>28</v>
       </c>
-      <c r="E11" s="32">
+      <c r="E11" s="26">
         <v>27</v>
       </c>
-      <c r="F11" s="33">
+      <c r="F11" s="27">
         <v>27</v>
       </c>
-      <c r="G11" s="34">
+      <c r="G11" s="28">
         <v>19</v>
       </c>
     </row>
@@ -1693,19 +1668,19 @@
       <c r="B12" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="C12" s="32">
+      <c r="C12" s="26">
         <v>1</v>
       </c>
-      <c r="D12" s="32">
-        <v>0</v>
-      </c>
-      <c r="E12" s="32">
+      <c r="D12" s="26">
+        <v>0</v>
+      </c>
+      <c r="E12" s="26">
         <v>1</v>
       </c>
-      <c r="F12" s="33">
+      <c r="F12" s="27">
         <v>1</v>
       </c>
-      <c r="G12" s="34">
+      <c r="G12" s="28">
         <v>2</v>
       </c>
     </row>
@@ -1716,19 +1691,19 @@
       <c r="B13" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="C13" s="32">
+      <c r="C13" s="26">
         <v>621</v>
       </c>
-      <c r="D13" s="32">
+      <c r="D13" s="26">
         <v>952</v>
       </c>
-      <c r="E13" s="32">
+      <c r="E13" s="26">
         <v>1061</v>
       </c>
-      <c r="F13" s="33">
+      <c r="F13" s="27">
         <v>1446</v>
       </c>
-      <c r="G13" s="34">
+      <c r="G13" s="28">
         <v>1470</v>
       </c>
     </row>
@@ -1739,19 +1714,19 @@
       <c r="B14" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="C14" s="32">
+      <c r="C14" s="26">
         <v>6</v>
       </c>
-      <c r="D14" s="32">
+      <c r="D14" s="26">
         <v>14</v>
       </c>
-      <c r="E14" s="32">
+      <c r="E14" s="26">
         <v>10</v>
       </c>
-      <c r="F14" s="33">
+      <c r="F14" s="27">
         <v>11</v>
       </c>
-      <c r="G14" s="35">
+      <c r="G14" s="29">
         <v>15</v>
       </c>
     </row>
@@ -1762,19 +1737,19 @@
       <c r="B15" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="C15" s="32">
+      <c r="C15" s="26">
         <v>168</v>
       </c>
-      <c r="D15" s="32">
+      <c r="D15" s="26">
         <v>42</v>
       </c>
-      <c r="E15" s="32">
+      <c r="E15" s="26">
         <v>15</v>
       </c>
-      <c r="F15" s="33">
+      <c r="F15" s="27">
         <v>9</v>
       </c>
-      <c r="G15" s="34">
+      <c r="G15" s="28">
         <v>3</v>
       </c>
     </row>
@@ -1785,19 +1760,19 @@
       <c r="B16" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="C16" s="32">
+      <c r="C16" s="26">
         <v>171</v>
       </c>
-      <c r="D16" s="32">
+      <c r="D16" s="26">
         <v>123</v>
       </c>
-      <c r="E16" s="32">
+      <c r="E16" s="26">
         <v>119</v>
       </c>
-      <c r="F16" s="33">
+      <c r="F16" s="27">
         <v>125</v>
       </c>
-      <c r="G16" s="34">
+      <c r="G16" s="28">
         <v>119</v>
       </c>
     </row>
@@ -1808,19 +1783,19 @@
       <c r="B17" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="C17" s="32">
+      <c r="C17" s="26">
         <v>81</v>
       </c>
-      <c r="D17" s="32">
+      <c r="D17" s="26">
         <v>202</v>
       </c>
-      <c r="E17" s="32">
+      <c r="E17" s="26">
         <v>88</v>
       </c>
-      <c r="F17" s="33">
+      <c r="F17" s="27">
         <v>69</v>
       </c>
-      <c r="G17" s="34">
+      <c r="G17" s="28">
         <v>31</v>
       </c>
     </row>
@@ -1831,19 +1806,19 @@
       <c r="B18" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="C18" s="32">
+      <c r="C18" s="26">
         <v>2</v>
       </c>
-      <c r="D18" s="32">
+      <c r="D18" s="26">
         <v>1</v>
       </c>
-      <c r="E18" s="32">
-        <v>0</v>
-      </c>
-      <c r="F18" s="33">
-        <v>0</v>
-      </c>
-      <c r="G18" s="34">
+      <c r="E18" s="26">
+        <v>0</v>
+      </c>
+      <c r="F18" s="27">
+        <v>0</v>
+      </c>
+      <c r="G18" s="28">
         <v>0</v>
       </c>
     </row>
@@ -1854,19 +1829,19 @@
       <c r="B19" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="C19" s="32">
+      <c r="C19" s="26">
         <v>105</v>
       </c>
-      <c r="D19" s="32">
+      <c r="D19" s="26">
         <v>45</v>
       </c>
-      <c r="E19" s="32">
+      <c r="E19" s="26">
         <v>87</v>
       </c>
-      <c r="F19" s="33">
+      <c r="F19" s="27">
         <v>47</v>
       </c>
-      <c r="G19" s="34">
+      <c r="G19" s="28">
         <v>51</v>
       </c>
     </row>
@@ -1877,19 +1852,19 @@
       <c r="B20" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="C20" s="32">
+      <c r="C20" s="26">
         <v>10</v>
       </c>
-      <c r="D20" s="32">
+      <c r="D20" s="26">
         <v>13</v>
       </c>
-      <c r="E20" s="32">
+      <c r="E20" s="26">
         <v>2</v>
       </c>
-      <c r="F20" s="33">
+      <c r="F20" s="27">
         <v>3</v>
       </c>
-      <c r="G20" s="34">
+      <c r="G20" s="28">
         <v>6</v>
       </c>
     </row>
@@ -1900,19 +1875,19 @@
       <c r="B21" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="C21" s="32">
+      <c r="C21" s="26">
         <v>1</v>
       </c>
-      <c r="D21" s="32">
+      <c r="D21" s="26">
         <v>7</v>
       </c>
-      <c r="E21" s="32">
+      <c r="E21" s="26">
         <v>4</v>
       </c>
-      <c r="F21" s="33">
+      <c r="F21" s="27">
         <v>2</v>
       </c>
-      <c r="G21" s="34">
+      <c r="G21" s="28">
         <v>4</v>
       </c>
     </row>
@@ -1923,19 +1898,19 @@
       <c r="B22" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="C22" s="32">
+      <c r="C22" s="26">
         <v>2</v>
       </c>
-      <c r="D22" s="32">
-        <v>0</v>
-      </c>
-      <c r="E22" s="32">
+      <c r="D22" s="26">
+        <v>0</v>
+      </c>
+      <c r="E22" s="26">
         <v>1</v>
       </c>
-      <c r="F22" s="33">
-        <v>0</v>
-      </c>
-      <c r="G22" s="34">
+      <c r="F22" s="27">
+        <v>0</v>
+      </c>
+      <c r="G22" s="28">
         <v>0</v>
       </c>
     </row>
@@ -1946,19 +1921,19 @@
       <c r="B23" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="C23" s="32">
+      <c r="C23" s="26">
         <v>23</v>
       </c>
-      <c r="D23" s="32">
+      <c r="D23" s="26">
         <v>41</v>
       </c>
-      <c r="E23" s="32">
+      <c r="E23" s="26">
         <v>55</v>
       </c>
-      <c r="F23" s="33">
-        <v>74</v>
-      </c>
-      <c r="G23" s="34">
+      <c r="F23" s="27">
+        <v>74</v>
+      </c>
+      <c r="G23" s="28">
         <v>15</v>
       </c>
     </row>
@@ -1969,19 +1944,19 @@
       <c r="B24" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="C24" s="32">
+      <c r="C24" s="26">
         <v>1</v>
       </c>
-      <c r="D24" s="32">
+      <c r="D24" s="26">
         <v>2</v>
       </c>
-      <c r="E24" s="32">
-        <v>0</v>
-      </c>
-      <c r="F24" s="33">
+      <c r="E24" s="26">
+        <v>0</v>
+      </c>
+      <c r="F24" s="27">
         <v>3</v>
       </c>
-      <c r="G24" s="34">
+      <c r="G24" s="28">
         <v>1</v>
       </c>
     </row>
@@ -1992,19 +1967,19 @@
       <c r="B25" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="C25" s="32">
+      <c r="C25" s="26">
         <v>3</v>
       </c>
-      <c r="D25" s="32">
-        <v>0</v>
-      </c>
-      <c r="E25" s="32">
+      <c r="D25" s="26">
+        <v>0</v>
+      </c>
+      <c r="E25" s="26">
         <v>1</v>
       </c>
-      <c r="F25" s="33">
+      <c r="F25" s="27">
         <v>2</v>
       </c>
-      <c r="G25" s="34">
+      <c r="G25" s="28">
         <v>9</v>
       </c>
     </row>
@@ -2015,19 +1990,19 @@
       <c r="B26" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="C26" s="32">
+      <c r="C26" s="26">
         <v>1</v>
       </c>
-      <c r="D26" s="32">
+      <c r="D26" s="26">
         <v>1</v>
       </c>
-      <c r="E26" s="32">
+      <c r="E26" s="26">
         <v>3</v>
       </c>
-      <c r="F26" s="33">
+      <c r="F26" s="27">
         <v>1</v>
       </c>
-      <c r="G26" s="34">
+      <c r="G26" s="28">
         <v>1</v>
       </c>
     </row>
@@ -2038,19 +2013,19 @@
       <c r="B27" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="C27" s="32">
+      <c r="C27" s="26">
         <v>92</v>
       </c>
-      <c r="D27" s="32">
+      <c r="D27" s="26">
         <v>176</v>
       </c>
-      <c r="E27" s="32">
+      <c r="E27" s="26">
         <v>236</v>
       </c>
-      <c r="F27" s="33">
+      <c r="F27" s="27">
         <v>189</v>
       </c>
-      <c r="G27" s="34">
+      <c r="G27" s="28">
         <v>73</v>
       </c>
     </row>
@@ -2061,19 +2036,19 @@
       <c r="B28" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="C28" s="32">
+      <c r="C28" s="26">
         <v>466</v>
       </c>
-      <c r="D28" s="32">
+      <c r="D28" s="26">
         <v>729</v>
       </c>
-      <c r="E28" s="32">
+      <c r="E28" s="26">
         <v>633</v>
       </c>
-      <c r="F28" s="33">
+      <c r="F28" s="27">
         <v>505</v>
       </c>
-      <c r="G28" s="34">
+      <c r="G28" s="28">
         <v>622</v>
       </c>
     </row>
@@ -2084,19 +2059,19 @@
       <c r="B29" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="C29" s="32">
+      <c r="C29" s="26">
         <v>449</v>
       </c>
-      <c r="D29" s="32">
+      <c r="D29" s="26">
         <v>718</v>
       </c>
-      <c r="E29" s="32">
+      <c r="E29" s="26">
         <v>438</v>
       </c>
-      <c r="F29" s="33">
+      <c r="F29" s="27">
         <v>418</v>
       </c>
-      <c r="G29" s="34">
+      <c r="G29" s="28">
         <v>566</v>
       </c>
     </row>
@@ -2107,19 +2082,19 @@
       <c r="B30" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="C30" s="32">
+      <c r="C30" s="26">
         <v>5</v>
       </c>
-      <c r="D30" s="32">
+      <c r="D30" s="26">
         <v>5</v>
       </c>
-      <c r="E30" s="32">
+      <c r="E30" s="26">
         <v>8</v>
       </c>
-      <c r="F30" s="33">
+      <c r="F30" s="27">
         <v>3</v>
       </c>
-      <c r="G30" s="34">
+      <c r="G30" s="28">
         <v>1</v>
       </c>
     </row>
@@ -2130,19 +2105,19 @@
       <c r="B31" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="C31" s="32">
+      <c r="C31" s="26">
         <v>3291</v>
       </c>
-      <c r="D31" s="32">
+      <c r="D31" s="26">
         <v>3326</v>
       </c>
-      <c r="E31" s="32">
+      <c r="E31" s="26">
         <v>3467</v>
       </c>
-      <c r="F31" s="33">
+      <c r="F31" s="27">
         <v>5789</v>
       </c>
-      <c r="G31" s="34">
+      <c r="G31" s="28">
         <v>6576</v>
       </c>
     </row>
@@ -2153,19 +2128,19 @@
       <c r="B32" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="C32" s="32">
-        <v>0</v>
-      </c>
-      <c r="D32" s="32">
-        <v>0</v>
-      </c>
-      <c r="E32" s="32">
+      <c r="C32" s="26">
+        <v>0</v>
+      </c>
+      <c r="D32" s="26">
+        <v>0</v>
+      </c>
+      <c r="E32" s="26">
         <v>1</v>
       </c>
-      <c r="F32" s="33">
+      <c r="F32" s="27">
         <v>2</v>
       </c>
-      <c r="G32" s="34">
+      <c r="G32" s="28">
         <v>1</v>
       </c>
     </row>
@@ -2176,19 +2151,19 @@
       <c r="B33" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="C33" s="32">
+      <c r="C33" s="26">
         <v>133</v>
       </c>
-      <c r="D33" s="32">
+      <c r="D33" s="26">
         <v>148</v>
       </c>
-      <c r="E33" s="32">
+      <c r="E33" s="26">
         <v>121</v>
       </c>
-      <c r="F33" s="33">
+      <c r="F33" s="27">
         <v>157</v>
       </c>
-      <c r="G33" s="34">
+      <c r="G33" s="28">
         <v>111</v>
       </c>
     </row>
@@ -2199,19 +2174,19 @@
       <c r="B34" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="C34" s="32">
-        <v>0</v>
-      </c>
-      <c r="D34" s="32">
-        <v>0</v>
-      </c>
-      <c r="E34" s="32">
-        <v>0</v>
-      </c>
-      <c r="F34" s="33">
+      <c r="C34" s="26">
+        <v>0</v>
+      </c>
+      <c r="D34" s="26">
+        <v>0</v>
+      </c>
+      <c r="E34" s="26">
+        <v>0</v>
+      </c>
+      <c r="F34" s="27">
         <v>1</v>
       </c>
-      <c r="G34" s="34">
+      <c r="G34" s="28">
         <v>1</v>
       </c>
     </row>
@@ -2222,19 +2197,19 @@
       <c r="B35" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="C35" s="32">
-        <v>0</v>
-      </c>
-      <c r="D35" s="32">
-        <v>0</v>
-      </c>
-      <c r="E35" s="32">
+      <c r="C35" s="26">
+        <v>0</v>
+      </c>
+      <c r="D35" s="26">
+        <v>0</v>
+      </c>
+      <c r="E35" s="26">
         <v>3</v>
       </c>
-      <c r="F35" s="33">
+      <c r="F35" s="27">
         <v>1</v>
       </c>
-      <c r="G35" s="34">
+      <c r="G35" s="28">
         <v>10</v>
       </c>
     </row>
@@ -2245,19 +2220,19 @@
       <c r="B36" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="C36" s="32">
+      <c r="C36" s="26">
         <v>123</v>
       </c>
-      <c r="D36" s="32">
+      <c r="D36" s="26">
         <v>54</v>
       </c>
-      <c r="E36" s="32">
+      <c r="E36" s="26">
         <v>51</v>
       </c>
-      <c r="F36" s="33">
+      <c r="F36" s="27">
         <v>90</v>
       </c>
-      <c r="G36" s="34">
+      <c r="G36" s="28">
         <v>139</v>
       </c>
     </row>
@@ -2268,42 +2243,42 @@
       <c r="B37" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="C37" s="32">
+      <c r="C37" s="26">
         <v>60</v>
       </c>
-      <c r="D37" s="32">
+      <c r="D37" s="26">
         <v>51</v>
       </c>
-      <c r="E37" s="32">
+      <c r="E37" s="26">
         <v>54</v>
       </c>
-      <c r="F37" s="33">
+      <c r="F37" s="27">
         <v>75</v>
       </c>
-      <c r="G37" s="34">
+      <c r="G37" s="28">
         <v>112</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A38" s="53" t="s">
+      <c r="A38" s="47" t="s">
         <v>102</v>
       </c>
       <c r="B38" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="C38" s="32">
-        <v>0</v>
-      </c>
-      <c r="D38" s="32">
-        <v>0</v>
-      </c>
-      <c r="E38" s="32">
-        <v>0</v>
-      </c>
-      <c r="F38" s="33">
-        <v>0</v>
-      </c>
-      <c r="G38" s="34">
+      <c r="C38" s="26">
+        <v>0</v>
+      </c>
+      <c r="D38" s="26">
+        <v>0</v>
+      </c>
+      <c r="E38" s="26">
+        <v>0</v>
+      </c>
+      <c r="F38" s="27">
+        <v>0</v>
+      </c>
+      <c r="G38" s="28">
         <v>0</v>
       </c>
     </row>
@@ -2314,19 +2289,19 @@
       <c r="B39" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="C39" s="32">
+      <c r="C39" s="26">
         <v>30</v>
       </c>
-      <c r="D39" s="32">
+      <c r="D39" s="26">
         <v>16</v>
       </c>
-      <c r="E39" s="32">
+      <c r="E39" s="26">
         <v>106</v>
       </c>
-      <c r="F39" s="33">
+      <c r="F39" s="27">
         <v>61</v>
       </c>
-      <c r="G39" s="34">
+      <c r="G39" s="28">
         <v>551</v>
       </c>
     </row>
@@ -2337,19 +2312,19 @@
       <c r="B40" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="C40" s="32">
-        <v>0</v>
-      </c>
-      <c r="D40" s="32">
-        <v>0</v>
-      </c>
-      <c r="E40" s="32">
+      <c r="C40" s="26">
+        <v>0</v>
+      </c>
+      <c r="D40" s="26">
+        <v>0</v>
+      </c>
+      <c r="E40" s="26">
         <v>9</v>
       </c>
-      <c r="F40" s="33">
+      <c r="F40" s="27">
         <v>12</v>
       </c>
-      <c r="G40" s="34">
+      <c r="G40" s="28">
         <v>7</v>
       </c>
     </row>
@@ -2377,25 +2352,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="C1" s="10" t="s">
+      <c r="C1" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="D1" s="10" t="s">
+      <c r="D1" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="E1" s="10" t="s">
+      <c r="E1" s="9" t="s">
         <v>56</v>
       </c>
-      <c r="F1" s="11" t="s">
+      <c r="F1" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="G1" s="8" t="s">
+      <c r="G1" s="7" t="s">
         <v>58</v>
       </c>
     </row>
@@ -2406,19 +2381,19 @@
       <c r="B2" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="C2" s="32">
+      <c r="C2" s="26">
         <v>6</v>
       </c>
-      <c r="D2" s="32">
+      <c r="D2" s="26">
         <v>6</v>
       </c>
-      <c r="E2" s="32">
+      <c r="E2" s="26">
         <v>8</v>
       </c>
-      <c r="F2" s="33">
+      <c r="F2" s="27">
         <v>7</v>
       </c>
-      <c r="G2" s="34">
+      <c r="G2" s="28">
         <v>8</v>
       </c>
     </row>
@@ -2429,19 +2404,19 @@
       <c r="B3" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="C3" s="32">
+      <c r="C3" s="26">
         <v>195</v>
       </c>
-      <c r="D3" s="32">
+      <c r="D3" s="26">
         <v>237</v>
       </c>
-      <c r="E3" s="32">
+      <c r="E3" s="26">
         <v>178</v>
       </c>
-      <c r="F3" s="33">
+      <c r="F3" s="27">
         <v>241</v>
       </c>
-      <c r="G3" s="34">
+      <c r="G3" s="28">
         <v>354</v>
       </c>
     </row>
@@ -2452,19 +2427,19 @@
       <c r="B4" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="C4" s="32">
+      <c r="C4" s="26">
         <v>1</v>
       </c>
-      <c r="D4" s="32">
+      <c r="D4" s="26">
         <v>9</v>
       </c>
-      <c r="E4" s="32">
+      <c r="E4" s="26">
         <v>5</v>
       </c>
-      <c r="F4" s="33">
+      <c r="F4" s="27">
         <v>4</v>
       </c>
-      <c r="G4" s="34">
+      <c r="G4" s="28">
         <v>6</v>
       </c>
     </row>
@@ -2475,65 +2450,65 @@
       <c r="B5" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="C5" s="32">
+      <c r="C5" s="26">
         <v>60</v>
       </c>
-      <c r="D5" s="32">
+      <c r="D5" s="26">
         <v>68</v>
       </c>
-      <c r="E5" s="32">
+      <c r="E5" s="26">
         <v>54</v>
       </c>
-      <c r="F5" s="33">
+      <c r="F5" s="27">
         <v>82</v>
       </c>
-      <c r="G5" s="34">
+      <c r="G5" s="28">
         <v>135</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="53" t="s">
+      <c r="A6" s="47" t="s">
         <v>63</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="C6" s="32">
+      <c r="C6" s="26">
         <v>27</v>
       </c>
-      <c r="D6" s="32">
+      <c r="D6" s="26">
         <v>25</v>
       </c>
-      <c r="E6" s="32">
+      <c r="E6" s="26">
         <v>12</v>
       </c>
-      <c r="F6" s="33">
+      <c r="F6" s="27">
         <v>6</v>
       </c>
-      <c r="G6" s="34">
+      <c r="G6" s="28">
         <v>2</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="53" t="s">
+      <c r="A7" s="47" t="s">
         <v>65</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="C7" s="32">
+      <c r="C7" s="26">
         <v>1</v>
       </c>
-      <c r="D7" s="32">
-        <v>0</v>
-      </c>
-      <c r="E7" s="32">
-        <v>0</v>
-      </c>
-      <c r="F7" s="33">
+      <c r="D7" s="26">
+        <v>0</v>
+      </c>
+      <c r="E7" s="26">
+        <v>0</v>
+      </c>
+      <c r="F7" s="27">
         <v>1</v>
       </c>
-      <c r="G7" s="34">
+      <c r="G7" s="28">
         <v>3</v>
       </c>
     </row>
@@ -2544,19 +2519,19 @@
       <c r="B8" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="C8" s="32">
+      <c r="C8" s="26">
         <v>48</v>
       </c>
-      <c r="D8" s="32">
+      <c r="D8" s="26">
         <v>33</v>
       </c>
-      <c r="E8" s="32">
+      <c r="E8" s="26">
         <v>34</v>
       </c>
-      <c r="F8" s="33">
+      <c r="F8" s="27">
         <v>38</v>
       </c>
-      <c r="G8" s="34">
+      <c r="G8" s="28">
         <v>22</v>
       </c>
     </row>
@@ -2567,19 +2542,19 @@
       <c r="B9" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="C9" s="32">
+      <c r="C9" s="26">
         <v>6554</v>
       </c>
-      <c r="D9" s="32">
+      <c r="D9" s="26">
         <v>11327</v>
       </c>
-      <c r="E9" s="32">
+      <c r="E9" s="26">
         <v>13815</v>
       </c>
-      <c r="F9" s="33">
+      <c r="F9" s="27">
         <v>11784</v>
       </c>
-      <c r="G9" s="34">
+      <c r="G9" s="28">
         <v>14295</v>
       </c>
     </row>
@@ -2590,19 +2565,19 @@
       <c r="B10" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="C10" s="32">
+      <c r="C10" s="26">
         <v>136</v>
       </c>
-      <c r="D10" s="32">
+      <c r="D10" s="26">
         <v>233</v>
       </c>
-      <c r="E10" s="32">
+      <c r="E10" s="26">
         <v>43</v>
       </c>
-      <c r="F10" s="33">
+      <c r="F10" s="27">
         <v>15</v>
       </c>
-      <c r="G10" s="34">
+      <c r="G10" s="28">
         <v>13</v>
       </c>
     </row>
@@ -2613,19 +2588,19 @@
       <c r="B11" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="C11" s="32">
+      <c r="C11" s="26">
         <v>34</v>
       </c>
-      <c r="D11" s="32">
+      <c r="D11" s="26">
         <v>28</v>
       </c>
-      <c r="E11" s="32">
+      <c r="E11" s="26">
         <v>27</v>
       </c>
-      <c r="F11" s="33">
+      <c r="F11" s="27">
         <v>27</v>
       </c>
-      <c r="G11" s="34">
+      <c r="G11" s="28">
         <v>19</v>
       </c>
     </row>
@@ -2636,19 +2611,19 @@
       <c r="B12" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="C12" s="32">
+      <c r="C12" s="26">
         <v>1</v>
       </c>
-      <c r="D12" s="32">
-        <v>0</v>
-      </c>
-      <c r="E12" s="32">
+      <c r="D12" s="26">
+        <v>0</v>
+      </c>
+      <c r="E12" s="26">
         <v>1</v>
       </c>
-      <c r="F12" s="33">
+      <c r="F12" s="27">
         <v>1</v>
       </c>
-      <c r="G12" s="34">
+      <c r="G12" s="28">
         <v>2</v>
       </c>
     </row>
@@ -2659,19 +2634,19 @@
       <c r="B13" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="C13" s="32">
+      <c r="C13" s="26">
         <v>621</v>
       </c>
-      <c r="D13" s="32">
+      <c r="D13" s="26">
         <v>952</v>
       </c>
-      <c r="E13" s="32">
+      <c r="E13" s="26">
         <v>1061</v>
       </c>
-      <c r="F13" s="33">
+      <c r="F13" s="27">
         <v>1446</v>
       </c>
-      <c r="G13" s="34">
+      <c r="G13" s="28">
         <v>1470</v>
       </c>
     </row>
@@ -2682,19 +2657,19 @@
       <c r="B14" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="C14" s="32">
+      <c r="C14" s="26">
         <v>6</v>
       </c>
-      <c r="D14" s="32">
+      <c r="D14" s="26">
         <v>14</v>
       </c>
-      <c r="E14" s="32">
+      <c r="E14" s="26">
         <v>10</v>
       </c>
-      <c r="F14" s="33">
+      <c r="F14" s="27">
         <v>11</v>
       </c>
-      <c r="G14" s="35">
+      <c r="G14" s="29">
         <v>15</v>
       </c>
     </row>
@@ -2705,19 +2680,19 @@
       <c r="B15" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="C15" s="32">
+      <c r="C15" s="26">
         <v>168</v>
       </c>
-      <c r="D15" s="32">
+      <c r="D15" s="26">
         <v>42</v>
       </c>
-      <c r="E15" s="32">
+      <c r="E15" s="26">
         <v>15</v>
       </c>
-      <c r="F15" s="33">
+      <c r="F15" s="27">
         <v>9</v>
       </c>
-      <c r="G15" s="34">
+      <c r="G15" s="28">
         <v>3</v>
       </c>
     </row>
@@ -2728,19 +2703,19 @@
       <c r="B16" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="C16" s="32">
+      <c r="C16" s="26">
         <v>171</v>
       </c>
-      <c r="D16" s="32">
+      <c r="D16" s="26">
         <v>123</v>
       </c>
-      <c r="E16" s="32">
+      <c r="E16" s="26">
         <v>119</v>
       </c>
-      <c r="F16" s="33">
+      <c r="F16" s="27">
         <v>125</v>
       </c>
-      <c r="G16" s="34">
+      <c r="G16" s="28">
         <v>119</v>
       </c>
     </row>
@@ -2751,19 +2726,19 @@
       <c r="B17" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="C17" s="32">
+      <c r="C17" s="26">
         <v>81</v>
       </c>
-      <c r="D17" s="32">
+      <c r="D17" s="26">
         <v>202</v>
       </c>
-      <c r="E17" s="32">
+      <c r="E17" s="26">
         <v>88</v>
       </c>
-      <c r="F17" s="33">
+      <c r="F17" s="27">
         <v>69</v>
       </c>
-      <c r="G17" s="34">
+      <c r="G17" s="28">
         <v>31</v>
       </c>
     </row>
@@ -2774,19 +2749,19 @@
       <c r="B18" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="C18" s="32">
+      <c r="C18" s="26">
         <v>2</v>
       </c>
-      <c r="D18" s="32">
+      <c r="D18" s="26">
         <v>1</v>
       </c>
-      <c r="E18" s="32">
-        <v>0</v>
-      </c>
-      <c r="F18" s="33">
-        <v>0</v>
-      </c>
-      <c r="G18" s="34">
+      <c r="E18" s="26">
+        <v>0</v>
+      </c>
+      <c r="F18" s="27">
+        <v>0</v>
+      </c>
+      <c r="G18" s="28">
         <v>0</v>
       </c>
     </row>
@@ -2797,19 +2772,19 @@
       <c r="B19" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="C19" s="32">
+      <c r="C19" s="26">
         <v>105</v>
       </c>
-      <c r="D19" s="32">
+      <c r="D19" s="26">
         <v>45</v>
       </c>
-      <c r="E19" s="32">
+      <c r="E19" s="26">
         <v>87</v>
       </c>
-      <c r="F19" s="33">
+      <c r="F19" s="27">
         <v>47</v>
       </c>
-      <c r="G19" s="34">
+      <c r="G19" s="28">
         <v>51</v>
       </c>
     </row>
@@ -2820,19 +2795,19 @@
       <c r="B20" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="C20" s="32">
+      <c r="C20" s="26">
         <v>10</v>
       </c>
-      <c r="D20" s="32">
+      <c r="D20" s="26">
         <v>13</v>
       </c>
-      <c r="E20" s="32">
+      <c r="E20" s="26">
         <v>2</v>
       </c>
-      <c r="F20" s="33">
+      <c r="F20" s="27">
         <v>3</v>
       </c>
-      <c r="G20" s="34">
+      <c r="G20" s="28">
         <v>6</v>
       </c>
     </row>
@@ -2843,19 +2818,19 @@
       <c r="B21" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="C21" s="32">
+      <c r="C21" s="26">
         <v>1</v>
       </c>
-      <c r="D21" s="32">
+      <c r="D21" s="26">
         <v>7</v>
       </c>
-      <c r="E21" s="32">
+      <c r="E21" s="26">
         <v>4</v>
       </c>
-      <c r="F21" s="33">
+      <c r="F21" s="27">
         <v>2</v>
       </c>
-      <c r="G21" s="34">
+      <c r="G21" s="28">
         <v>4</v>
       </c>
     </row>
@@ -2866,19 +2841,19 @@
       <c r="B22" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="C22" s="32">
+      <c r="C22" s="26">
         <v>2</v>
       </c>
-      <c r="D22" s="32">
-        <v>0</v>
-      </c>
-      <c r="E22" s="32">
+      <c r="D22" s="26">
+        <v>0</v>
+      </c>
+      <c r="E22" s="26">
         <v>1</v>
       </c>
-      <c r="F22" s="33">
-        <v>0</v>
-      </c>
-      <c r="G22" s="34">
+      <c r="F22" s="27">
+        <v>0</v>
+      </c>
+      <c r="G22" s="28">
         <v>0</v>
       </c>
     </row>
@@ -2889,19 +2864,19 @@
       <c r="B23" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="C23" s="32">
+      <c r="C23" s="26">
         <v>23</v>
       </c>
-      <c r="D23" s="32">
+      <c r="D23" s="26">
         <v>41</v>
       </c>
-      <c r="E23" s="32">
+      <c r="E23" s="26">
         <v>55</v>
       </c>
-      <c r="F23" s="33">
-        <v>74</v>
-      </c>
-      <c r="G23" s="34">
+      <c r="F23" s="27">
+        <v>74</v>
+      </c>
+      <c r="G23" s="28">
         <v>15</v>
       </c>
     </row>
@@ -2912,19 +2887,19 @@
       <c r="B24" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="C24" s="32">
+      <c r="C24" s="26">
         <v>1</v>
       </c>
-      <c r="D24" s="32">
+      <c r="D24" s="26">
         <v>2</v>
       </c>
-      <c r="E24" s="32">
-        <v>0</v>
-      </c>
-      <c r="F24" s="33">
+      <c r="E24" s="26">
+        <v>0</v>
+      </c>
+      <c r="F24" s="27">
         <v>3</v>
       </c>
-      <c r="G24" s="34">
+      <c r="G24" s="28">
         <v>1</v>
       </c>
     </row>
@@ -2935,19 +2910,19 @@
       <c r="B25" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="C25" s="32">
+      <c r="C25" s="26">
         <v>3</v>
       </c>
-      <c r="D25" s="32">
-        <v>0</v>
-      </c>
-      <c r="E25" s="32">
+      <c r="D25" s="26">
+        <v>0</v>
+      </c>
+      <c r="E25" s="26">
         <v>1</v>
       </c>
-      <c r="F25" s="33">
+      <c r="F25" s="27">
         <v>2</v>
       </c>
-      <c r="G25" s="34">
+      <c r="G25" s="28">
         <v>9</v>
       </c>
     </row>
@@ -2958,19 +2933,19 @@
       <c r="B26" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="C26" s="32">
+      <c r="C26" s="26">
         <v>1</v>
       </c>
-      <c r="D26" s="32">
+      <c r="D26" s="26">
         <v>1</v>
       </c>
-      <c r="E26" s="32">
+      <c r="E26" s="26">
         <v>3</v>
       </c>
-      <c r="F26" s="33">
+      <c r="F26" s="27">
         <v>1</v>
       </c>
-      <c r="G26" s="34">
+      <c r="G26" s="28">
         <v>1</v>
       </c>
     </row>
@@ -2981,19 +2956,19 @@
       <c r="B27" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="C27" s="32">
+      <c r="C27" s="26">
         <v>92</v>
       </c>
-      <c r="D27" s="32">
+      <c r="D27" s="26">
         <v>176</v>
       </c>
-      <c r="E27" s="32">
+      <c r="E27" s="26">
         <v>236</v>
       </c>
-      <c r="F27" s="33">
+      <c r="F27" s="27">
         <v>189</v>
       </c>
-      <c r="G27" s="34">
+      <c r="G27" s="28">
         <v>73</v>
       </c>
     </row>
@@ -3004,19 +2979,19 @@
       <c r="B28" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="C28" s="32">
+      <c r="C28" s="26">
         <v>466</v>
       </c>
-      <c r="D28" s="32">
+      <c r="D28" s="26">
         <v>729</v>
       </c>
-      <c r="E28" s="32">
+      <c r="E28" s="26">
         <v>633</v>
       </c>
-      <c r="F28" s="33">
+      <c r="F28" s="27">
         <v>505</v>
       </c>
-      <c r="G28" s="34">
+      <c r="G28" s="28">
         <v>622</v>
       </c>
     </row>
@@ -3027,19 +3002,19 @@
       <c r="B29" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="C29" s="32">
+      <c r="C29" s="26">
         <v>449</v>
       </c>
-      <c r="D29" s="32">
+      <c r="D29" s="26">
         <v>718</v>
       </c>
-      <c r="E29" s="32">
+      <c r="E29" s="26">
         <v>438</v>
       </c>
-      <c r="F29" s="33">
+      <c r="F29" s="27">
         <v>418</v>
       </c>
-      <c r="G29" s="34">
+      <c r="G29" s="28">
         <v>566</v>
       </c>
     </row>
@@ -3050,19 +3025,19 @@
       <c r="B30" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="C30" s="32">
+      <c r="C30" s="26">
         <v>5</v>
       </c>
-      <c r="D30" s="32">
+      <c r="D30" s="26">
         <v>5</v>
       </c>
-      <c r="E30" s="32">
+      <c r="E30" s="26">
         <v>8</v>
       </c>
-      <c r="F30" s="33">
+      <c r="F30" s="27">
         <v>3</v>
       </c>
-      <c r="G30" s="34">
+      <c r="G30" s="28">
         <v>1</v>
       </c>
     </row>
@@ -3073,19 +3048,19 @@
       <c r="B31" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="C31" s="32">
+      <c r="C31" s="26">
         <v>3291</v>
       </c>
-      <c r="D31" s="32">
+      <c r="D31" s="26">
         <v>3326</v>
       </c>
-      <c r="E31" s="32">
+      <c r="E31" s="26">
         <v>3467</v>
       </c>
-      <c r="F31" s="33">
+      <c r="F31" s="27">
         <v>5789</v>
       </c>
-      <c r="G31" s="34">
+      <c r="G31" s="28">
         <v>6576</v>
       </c>
     </row>
@@ -3096,19 +3071,19 @@
       <c r="B32" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="C32" s="32">
-        <v>0</v>
-      </c>
-      <c r="D32" s="32">
-        <v>0</v>
-      </c>
-      <c r="E32" s="32">
+      <c r="C32" s="26">
+        <v>0</v>
+      </c>
+      <c r="D32" s="26">
+        <v>0</v>
+      </c>
+      <c r="E32" s="26">
         <v>1</v>
       </c>
-      <c r="F32" s="33">
+      <c r="F32" s="27">
         <v>2</v>
       </c>
-      <c r="G32" s="34">
+      <c r="G32" s="28">
         <v>1</v>
       </c>
     </row>
@@ -3119,19 +3094,19 @@
       <c r="B33" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="C33" s="32">
+      <c r="C33" s="26">
         <v>133</v>
       </c>
-      <c r="D33" s="32">
+      <c r="D33" s="26">
         <v>148</v>
       </c>
-      <c r="E33" s="32">
+      <c r="E33" s="26">
         <v>121</v>
       </c>
-      <c r="F33" s="33">
+      <c r="F33" s="27">
         <v>157</v>
       </c>
-      <c r="G33" s="34">
+      <c r="G33" s="28">
         <v>111</v>
       </c>
     </row>
@@ -3142,19 +3117,19 @@
       <c r="B34" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="C34" s="32">
-        <v>0</v>
-      </c>
-      <c r="D34" s="32">
-        <v>0</v>
-      </c>
-      <c r="E34" s="32">
-        <v>0</v>
-      </c>
-      <c r="F34" s="33">
+      <c r="C34" s="26">
+        <v>0</v>
+      </c>
+      <c r="D34" s="26">
+        <v>0</v>
+      </c>
+      <c r="E34" s="26">
+        <v>0</v>
+      </c>
+      <c r="F34" s="27">
         <v>1</v>
       </c>
-      <c r="G34" s="34">
+      <c r="G34" s="28">
         <v>1</v>
       </c>
     </row>
@@ -3165,19 +3140,19 @@
       <c r="B35" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="C35" s="32">
-        <v>0</v>
-      </c>
-      <c r="D35" s="32">
-        <v>0</v>
-      </c>
-      <c r="E35" s="32">
+      <c r="C35" s="26">
+        <v>0</v>
+      </c>
+      <c r="D35" s="26">
+        <v>0</v>
+      </c>
+      <c r="E35" s="26">
         <v>3</v>
       </c>
-      <c r="F35" s="33">
+      <c r="F35" s="27">
         <v>1</v>
       </c>
-      <c r="G35" s="34">
+      <c r="G35" s="28">
         <v>10</v>
       </c>
     </row>
@@ -3188,19 +3163,19 @@
       <c r="B36" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="C36" s="32">
+      <c r="C36" s="26">
         <v>123</v>
       </c>
-      <c r="D36" s="32">
+      <c r="D36" s="26">
         <v>54</v>
       </c>
-      <c r="E36" s="32">
+      <c r="E36" s="26">
         <v>51</v>
       </c>
-      <c r="F36" s="33">
+      <c r="F36" s="27">
         <v>90</v>
       </c>
-      <c r="G36" s="34">
+      <c r="G36" s="28">
         <v>139</v>
       </c>
     </row>
@@ -3211,19 +3186,19 @@
       <c r="B37" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="C37" s="32">
+      <c r="C37" s="26">
         <v>60</v>
       </c>
-      <c r="D37" s="32">
+      <c r="D37" s="26">
         <v>51</v>
       </c>
-      <c r="E37" s="32">
+      <c r="E37" s="26">
         <v>54</v>
       </c>
-      <c r="F37" s="33">
+      <c r="F37" s="27">
         <v>75</v>
       </c>
-      <c r="G37" s="34">
+      <c r="G37" s="28">
         <v>112</v>
       </c>
     </row>
@@ -3234,19 +3209,19 @@
       <c r="B38" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="C38" s="32">
+      <c r="C38" s="26">
         <v>30</v>
       </c>
-      <c r="D38" s="32">
+      <c r="D38" s="26">
         <v>16</v>
       </c>
-      <c r="E38" s="32">
+      <c r="E38" s="26">
         <v>106</v>
       </c>
-      <c r="F38" s="33">
+      <c r="F38" s="27">
         <v>61</v>
       </c>
-      <c r="G38" s="34">
+      <c r="G38" s="28">
         <v>551</v>
       </c>
     </row>
@@ -3257,19 +3232,19 @@
       <c r="B39" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="C39" s="32">
-        <v>0</v>
-      </c>
-      <c r="D39" s="32">
-        <v>0</v>
-      </c>
-      <c r="E39" s="32">
+      <c r="C39" s="26">
+        <v>0</v>
+      </c>
+      <c r="D39" s="26">
+        <v>0</v>
+      </c>
+      <c r="E39" s="26">
         <v>9</v>
       </c>
-      <c r="F39" s="33">
+      <c r="F39" s="27">
         <v>12</v>
       </c>
-      <c r="G39" s="34">
+      <c r="G39" s="28">
         <v>7</v>
       </c>
     </row>
@@ -3292,120 +3267,120 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="12"/>
-    <col min="2" max="2" width="12.5703125" style="12" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.85546875" style="12" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.85546875" style="12" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19" style="12" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="29.85546875" style="12" bestFit="1" customWidth="1"/>
-    <col min="7" max="11" width="10.7109375" style="12" bestFit="1" customWidth="1"/>
-    <col min="12" max="16384" width="9.140625" style="12"/>
+    <col min="1" max="1" width="9.140625" style="11"/>
+    <col min="2" max="2" width="12.5703125" style="11" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.85546875" style="11" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.85546875" style="11" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19" style="11" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="29.85546875" style="11" bestFit="1" customWidth="1"/>
+    <col min="7" max="11" width="10.7109375" style="11" bestFit="1" customWidth="1"/>
+    <col min="12" max="16384" width="9.140625" style="11"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A1" s="12" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="12" t="s">
+      <c r="A1" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="12" t="s">
+      <c r="C1" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="D1" s="12" t="s">
+      <c r="D1" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="E1" s="12" t="s">
+      <c r="E1" s="11" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2" s="12">
+      <c r="A2" s="11">
         <v>2016</v>
       </c>
-      <c r="B2" s="22">
+      <c r="B2" s="17">
         <v>95314</v>
       </c>
-      <c r="C2" s="22">
+      <c r="C2" s="17">
         <v>117472</v>
       </c>
-      <c r="D2" s="22">
+      <c r="D2" s="17">
         <v>102940</v>
       </c>
-      <c r="E2" s="22">
+      <c r="E2" s="17">
         <v>14532</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A3" s="12">
+      <c r="A3" s="11">
         <v>2017</v>
       </c>
-      <c r="B3" s="22">
+      <c r="B3" s="17">
         <v>105300</v>
       </c>
-      <c r="C3" s="22">
+      <c r="C3" s="17">
         <v>126530</v>
       </c>
-      <c r="D3" s="22">
+      <c r="D3" s="17">
         <v>113634</v>
       </c>
-      <c r="E3" s="22">
+      <c r="E3" s="17">
         <v>12896</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A4" s="12">
+      <c r="A4" s="11">
         <v>2018</v>
       </c>
-      <c r="B4" s="22">
+      <c r="B4" s="17">
         <v>102457</v>
       </c>
-      <c r="C4" s="22">
+      <c r="C4" s="17">
         <v>126753</v>
       </c>
-      <c r="D4" s="22">
+      <c r="D4" s="17">
         <v>112218</v>
       </c>
-      <c r="E4" s="22">
+      <c r="E4" s="17">
         <v>14535</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A5" s="12">
+      <c r="A5" s="11">
         <v>2019</v>
       </c>
-      <c r="B5" s="22">
+      <c r="B5" s="17">
         <v>87522</v>
       </c>
-      <c r="C5" s="22">
+      <c r="C5" s="17">
         <v>115603</v>
       </c>
-      <c r="D5" s="22">
+      <c r="D5" s="17">
         <v>97908</v>
       </c>
-      <c r="E5" s="22">
+      <c r="E5" s="17">
         <v>17695</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A6" s="12">
+      <c r="A6" s="11">
         <v>2020</v>
       </c>
-      <c r="B6" s="22">
+      <c r="B6" s="17">
         <v>72918</v>
       </c>
-      <c r="C6" s="22">
+      <c r="C6" s="17">
         <v>99517</v>
       </c>
-      <c r="D6" s="22">
+      <c r="D6" s="17">
         <v>81309</v>
       </c>
-      <c r="E6" s="22">
+      <c r="E6" s="17">
         <v>18208</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="L10" s="23"/>
+      <c r="L10" s="18"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3417,10 +3392,10 @@
   <sheetPr>
     <tabColor rgb="FF00B050"/>
   </sheetPr>
-  <dimension ref="A1:Q19"/>
+  <dimension ref="A1:Q6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A7" sqref="A7:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3438,415 +3413,352 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A1" s="42" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="43" t="s">
+      <c r="A1" s="36" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="37" t="s">
         <v>22</v>
       </c>
-      <c r="C1" s="43" t="s">
+      <c r="C1" s="37" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="43" t="s">
+      <c r="D1" s="37" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="43" t="s">
+      <c r="E1" s="37" t="s">
         <v>23</v>
       </c>
-      <c r="F1" s="43" t="s">
+      <c r="F1" s="37" t="s">
         <v>24</v>
       </c>
-      <c r="G1" s="52" t="s">
+      <c r="G1" s="46" t="s">
         <v>25</v>
       </c>
-      <c r="H1" s="54" t="s">
+      <c r="H1" s="48" t="s">
         <v>26</v>
       </c>
-      <c r="I1" s="55" t="s">
+      <c r="I1" s="49" t="s">
         <v>27</v>
       </c>
-      <c r="J1" s="55" t="s">
+      <c r="J1" s="49" t="s">
         <v>28</v>
       </c>
-      <c r="K1" s="56" t="s">
+      <c r="K1" s="50" t="s">
         <v>29</v>
       </c>
-      <c r="L1" s="54" t="s">
+      <c r="L1" s="48" t="s">
         <v>30</v>
       </c>
-      <c r="M1" s="55" t="s">
+      <c r="M1" s="49" t="s">
         <v>31</v>
       </c>
-      <c r="N1" s="55" t="s">
+      <c r="N1" s="49" t="s">
         <v>32</v>
       </c>
-      <c r="O1" s="56" t="s">
+      <c r="O1" s="50" t="s">
         <v>33</v>
       </c>
-      <c r="P1" s="54" t="s">
+      <c r="P1" s="48" t="s">
         <v>34</v>
       </c>
-      <c r="Q1" s="56" t="s">
+      <c r="Q1" s="50" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A2" s="44">
+      <c r="A2" s="38">
         <v>2016</v>
       </c>
-      <c r="B2" s="38">
+      <c r="B2" s="32">
         <v>90331</v>
       </c>
-      <c r="C2" s="39">
+      <c r="C2" s="33">
         <v>12907</v>
       </c>
-      <c r="D2" s="39">
+      <c r="D2" s="33">
         <v>77418</v>
       </c>
-      <c r="E2" s="45">
+      <c r="E2" s="39">
         <v>64133</v>
       </c>
-      <c r="F2" s="45">
+      <c r="F2" s="39">
         <v>2268</v>
       </c>
-      <c r="G2" s="46">
+      <c r="G2" s="40">
         <v>11017</v>
       </c>
-      <c r="H2" s="57">
+      <c r="H2" s="51">
         <f>K2-I2</f>
         <v>-18140</v>
       </c>
-      <c r="I2" s="58">
+      <c r="I2" s="52">
         <v>43169</v>
       </c>
-      <c r="J2" s="59">
+      <c r="J2" s="53">
         <f>I2/(I2+M2)</f>
         <v>0.43418220586164585</v>
       </c>
-      <c r="K2" s="60">
+      <c r="K2" s="54">
         <v>25029</v>
       </c>
-      <c r="L2" s="44">
+      <c r="L2" s="38">
         <f>O2-M2</f>
         <v>8834</v>
       </c>
-      <c r="M2" s="58">
+      <c r="M2" s="52">
         <v>56257</v>
       </c>
-      <c r="N2" s="59">
+      <c r="N2" s="53">
         <f>M2/(M2+I2)</f>
         <v>0.5658177941383542</v>
       </c>
-      <c r="O2" s="62">
+      <c r="O2" s="56">
         <v>65091</v>
       </c>
-      <c r="P2" s="67">
+      <c r="P2" s="61">
         <f>K2/(K2+O2)</f>
         <v>0.27772969374167777</v>
       </c>
-      <c r="Q2" s="68">
+      <c r="Q2" s="62">
         <f>O2/(O2+K2)</f>
         <v>0.72227030625832223</v>
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A3" s="44">
+      <c r="A3" s="38">
         <v>2017</v>
       </c>
-      <c r="B3" s="38">
+      <c r="B3" s="32">
         <v>103650</v>
       </c>
-      <c r="C3" s="39">
+      <c r="C3" s="33">
         <v>18632</v>
       </c>
-      <c r="D3" s="39">
+      <c r="D3" s="33">
         <v>75018</v>
       </c>
-      <c r="E3" s="47">
+      <c r="E3" s="41">
         <v>57846</v>
       </c>
-      <c r="F3" s="47">
+      <c r="F3" s="41">
         <v>1732</v>
       </c>
-      <c r="G3" s="48">
+      <c r="G3" s="42">
         <v>15440</v>
       </c>
-      <c r="H3" s="57">
+      <c r="H3" s="51">
         <f>K3-I3</f>
         <v>-10237</v>
       </c>
-      <c r="I3" s="58">
+      <c r="I3" s="52">
         <v>40320</v>
       </c>
-      <c r="J3" s="59">
+      <c r="J3" s="53">
         <f t="shared" ref="J3:J6" si="0">I3/(I3+M3)</f>
         <v>0.49967159480995871</v>
       </c>
-      <c r="K3" s="60">
+      <c r="K3" s="54">
         <v>30083</v>
       </c>
-      <c r="L3" s="44">
+      <c r="L3" s="38">
         <f t="shared" ref="L3:L6" si="1">O3-M3</f>
         <v>16996</v>
       </c>
-      <c r="M3" s="58">
+      <c r="M3" s="52">
         <v>40373</v>
       </c>
-      <c r="N3" s="59">
+      <c r="N3" s="53">
         <f t="shared" ref="N3:N6" si="2">M3/(M3+I3)</f>
         <v>0.50032840519004129</v>
       </c>
-      <c r="O3" s="62">
+      <c r="O3" s="56">
         <v>57369</v>
       </c>
-      <c r="P3" s="67">
+      <c r="P3" s="61">
         <f>K3/(K3+O3)</f>
         <v>0.34399441979600237</v>
       </c>
-      <c r="Q3" s="68">
+      <c r="Q3" s="62">
         <f>O3/(O3+K3)</f>
         <v>0.65600558020399757</v>
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A4" s="44">
+      <c r="A4" s="38">
         <v>2018</v>
       </c>
-      <c r="B4" s="38">
+      <c r="B4" s="32">
         <v>101947</v>
       </c>
-      <c r="C4" s="39">
+      <c r="C4" s="33">
         <v>20750</v>
       </c>
-      <c r="D4" s="39">
+      <c r="D4" s="33">
         <v>80747</v>
       </c>
-      <c r="E4" s="47">
+      <c r="E4" s="41">
         <v>66324</v>
       </c>
-      <c r="F4" s="47">
+      <c r="F4" s="41">
         <v>238</v>
       </c>
-      <c r="G4" s="48">
+      <c r="G4" s="42">
         <v>14185</v>
       </c>
-      <c r="H4" s="61">
+      <c r="H4" s="55">
         <f>K4-I4</f>
         <v>4726</v>
       </c>
-      <c r="I4" s="58">
+      <c r="I4" s="52">
         <v>38443</v>
       </c>
-      <c r="J4" s="59">
+      <c r="J4" s="53">
         <f t="shared" si="0"/>
         <v>0.49905234188389241</v>
       </c>
-      <c r="K4" s="62">
+      <c r="K4" s="56">
         <v>43169</v>
       </c>
-      <c r="L4" s="44">
+      <c r="L4" s="38">
         <f t="shared" si="1"/>
         <v>17667</v>
       </c>
-      <c r="M4" s="58">
+      <c r="M4" s="52">
         <v>38589</v>
       </c>
-      <c r="N4" s="59">
+      <c r="N4" s="53">
         <f t="shared" si="2"/>
         <v>0.50094765811610764</v>
       </c>
-      <c r="O4" s="62">
+      <c r="O4" s="56">
         <v>56256</v>
       </c>
-      <c r="P4" s="67">
+      <c r="P4" s="61">
         <f>K4/(K4+O4)</f>
         <v>0.43418657279356299</v>
       </c>
-      <c r="Q4" s="68">
+      <c r="Q4" s="62">
         <f>O4/(O4+K4)</f>
         <v>0.56581342720643701</v>
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A5" s="44">
+      <c r="A5" s="38">
         <v>2019</v>
       </c>
-      <c r="B5" s="38">
+      <c r="B5" s="32">
         <v>93197</v>
       </c>
-      <c r="C5" s="39">
+      <c r="C5" s="33">
         <v>21301</v>
       </c>
-      <c r="D5" s="39">
+      <c r="D5" s="33">
         <v>71716</v>
       </c>
-      <c r="E5" s="47">
+      <c r="E5" s="41">
         <v>56243</v>
       </c>
-      <c r="F5" s="47">
+      <c r="F5" s="41">
         <v>234</v>
       </c>
-      <c r="G5" s="48">
+      <c r="G5" s="42">
         <v>15239</v>
       </c>
-      <c r="H5" s="61">
+      <c r="H5" s="55">
         <f>K5-I5</f>
         <v>861</v>
       </c>
-      <c r="I5" s="58">
+      <c r="I5" s="52">
         <v>44454</v>
       </c>
-      <c r="J5" s="59">
+      <c r="J5" s="53">
         <f>I5/(I5+M5)</f>
         <v>0.66956862272562956</v>
       </c>
-      <c r="K5" s="62">
+      <c r="K5" s="56">
         <v>45315</v>
       </c>
-      <c r="L5" s="44">
+      <c r="L5" s="38">
         <f t="shared" si="1"/>
         <v>20342</v>
       </c>
-      <c r="M5" s="58">
+      <c r="M5" s="52">
         <v>21938</v>
       </c>
-      <c r="N5" s="59">
+      <c r="N5" s="53">
         <f t="shared" si="2"/>
         <v>0.33043137727437039</v>
       </c>
-      <c r="O5" s="62">
+      <c r="O5" s="56">
         <v>42280</v>
       </c>
-      <c r="P5" s="67">
+      <c r="P5" s="61">
         <f>K5/(K5+O5)</f>
         <v>0.51732404817626576</v>
       </c>
-      <c r="Q5" s="68">
+      <c r="Q5" s="62">
         <f>O5/(O5+K5)</f>
         <v>0.48267595182373424</v>
       </c>
     </row>
     <row r="6" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="49">
+      <c r="A6" s="43">
         <v>2020</v>
       </c>
-      <c r="B6" s="40">
+      <c r="B6" s="34">
         <v>75137</v>
       </c>
-      <c r="C6" s="41">
+      <c r="C6" s="35">
         <v>25354</v>
       </c>
-      <c r="D6" s="41">
+      <c r="D6" s="35">
         <v>49783</v>
       </c>
-      <c r="E6" s="50">
+      <c r="E6" s="44">
         <v>38053</v>
       </c>
-      <c r="F6" s="50">
+      <c r="F6" s="44">
         <v>62</v>
       </c>
-      <c r="G6" s="51">
+      <c r="G6" s="45">
         <v>11668</v>
       </c>
-      <c r="H6" s="63">
+      <c r="H6" s="57">
         <f>K6-I6</f>
         <v>1509</v>
       </c>
-      <c r="I6" s="64">
+      <c r="I6" s="58">
         <v>35702</v>
       </c>
-      <c r="J6" s="65">
+      <c r="J6" s="59">
         <f t="shared" si="0"/>
         <v>0.74469150223186353</v>
       </c>
-      <c r="K6" s="66">
+      <c r="K6" s="60">
         <v>37211</v>
       </c>
-      <c r="L6" s="49">
+      <c r="L6" s="43">
         <f t="shared" si="1"/>
         <v>23720</v>
       </c>
-      <c r="M6" s="64">
+      <c r="M6" s="58">
         <v>12240</v>
       </c>
-      <c r="N6" s="65">
+      <c r="N6" s="59">
         <f t="shared" si="2"/>
         <v>0.25530849776813652</v>
       </c>
-      <c r="O6" s="66">
+      <c r="O6" s="60">
         <v>35960</v>
       </c>
-      <c r="P6" s="69">
+      <c r="P6" s="63">
         <f>K6/(K6+O6)</f>
         <v>0.50854846865561498</v>
       </c>
-      <c r="Q6" s="70">
+      <c r="Q6" s="64">
         <f>O6/(O6+K6)</f>
         <v>0.49145153134438507</v>
       </c>
-    </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="M7" s="19"/>
-      <c r="N7" s="19"/>
-      <c r="O7" s="19"/>
-    </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="H8" s="31"/>
-      <c r="I8" s="31"/>
-      <c r="J8" s="31"/>
-      <c r="P8" s="15"/>
-    </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="J9" s="4"/>
-      <c r="P9" s="16"/>
-    </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="P10" s="16"/>
-    </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="C11" s="15"/>
-      <c r="J11" s="14"/>
-      <c r="K11" s="15"/>
-      <c r="P11" s="16"/>
-    </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="J12" s="14"/>
-      <c r="P12" s="16"/>
-    </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="C13" s="71"/>
-      <c r="D13" s="71"/>
-      <c r="E13" s="71"/>
-      <c r="F13" s="71"/>
-      <c r="G13" s="71"/>
-      <c r="J13" s="14"/>
-      <c r="P13" s="13"/>
-    </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="J14" s="14"/>
-      <c r="P14" s="13"/>
-      <c r="Q14" s="4"/>
-    </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="C15" s="71"/>
-      <c r="E15" t="s">
-        <v>103</v>
-      </c>
-      <c r="J15" s="14"/>
-      <c r="P15" s="15"/>
-    </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="C16" s="71"/>
-      <c r="P16" s="15"/>
-    </row>
-    <row r="17" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C17" s="71"/>
-    </row>
-    <row r="18" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C18" s="71"/>
-    </row>
-    <row r="19" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C19" s="71"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3872,10 +3784,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="24" t="s">
+      <c r="B1" s="19" t="s">
         <v>0</v>
       </c>
       <c r="C1" t="s">
@@ -3883,332 +3795,332 @@
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="24" t="s">
+      <c r="A2" s="19" t="s">
         <v>11</v>
       </c>
       <c r="B2">
         <v>2016</v>
       </c>
-      <c r="C2" s="24">
+      <c r="C2" s="19">
         <v>95314</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="24" t="s">
+      <c r="A3" s="19" t="s">
         <v>12</v>
       </c>
       <c r="B3">
         <v>2016</v>
       </c>
-      <c r="C3" s="24">
+      <c r="C3" s="19">
         <v>14495</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="24" t="s">
+      <c r="A4" s="19" t="s">
         <v>13</v>
       </c>
       <c r="B4">
         <v>2016</v>
       </c>
-      <c r="C4" s="24">
+      <c r="C4" s="19">
         <v>4900</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="24" t="s">
+      <c r="A5" s="19" t="s">
         <v>14</v>
       </c>
       <c r="B5">
         <v>2016</v>
       </c>
-      <c r="C5" s="24">
+      <c r="C5" s="19">
         <v>2415</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="24" t="s">
+      <c r="A6" s="19" t="s">
         <v>15</v>
       </c>
       <c r="B6">
         <v>2016</v>
       </c>
-      <c r="C6" s="24">
+      <c r="C6" s="19">
         <v>264</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="24" t="s">
+      <c r="A7" s="19" t="s">
         <v>16</v>
       </c>
       <c r="B7">
         <v>2016</v>
       </c>
-      <c r="C7" s="24">
+      <c r="C7" s="19">
         <v>84</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="24" t="s">
+      <c r="A8" s="19" t="s">
         <v>11</v>
       </c>
       <c r="B8">
         <v>2017</v>
       </c>
-      <c r="C8" s="24">
+      <c r="C8" s="19">
         <v>105300</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="24" t="s">
+      <c r="A9" s="19" t="s">
         <v>12</v>
       </c>
       <c r="B9">
         <v>2017</v>
       </c>
-      <c r="C9" s="24">
+      <c r="C9" s="19">
         <v>12986</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="24" t="s">
+      <c r="A10" s="19" t="s">
         <v>13</v>
       </c>
       <c r="B10">
         <v>2017</v>
       </c>
-      <c r="C10" s="24">
+      <c r="C10" s="19">
         <v>4565</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="24" t="s">
+      <c r="A11" s="19" t="s">
         <v>14</v>
       </c>
       <c r="B11">
         <v>2017</v>
       </c>
-      <c r="C11" s="24">
+      <c r="C11" s="19">
         <v>3191</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="24" t="s">
+      <c r="A12" s="19" t="s">
         <v>15</v>
       </c>
       <c r="B12">
         <v>2017</v>
       </c>
-      <c r="C12" s="24">
+      <c r="C12" s="19">
         <v>398</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="24" t="s">
+      <c r="A13" s="19" t="s">
         <v>16</v>
       </c>
       <c r="B13">
         <v>2017</v>
       </c>
-      <c r="C13" s="24">
+      <c r="C13" s="19">
         <v>90</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="24" t="s">
+      <c r="A14" s="19" t="s">
         <v>11</v>
       </c>
       <c r="B14">
         <v>2018</v>
       </c>
-      <c r="C14" s="24">
+      <c r="C14" s="19">
         <v>102457</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="24" t="s">
+      <c r="A15" s="19" t="s">
         <v>12</v>
       </c>
       <c r="B15">
         <v>2018</v>
       </c>
-      <c r="C15" s="24">
+      <c r="C15" s="19">
         <v>15655</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="24" t="s">
+      <c r="A16" s="19" t="s">
         <v>13</v>
       </c>
       <c r="B16">
         <v>2018</v>
       </c>
-      <c r="C16" s="24">
+      <c r="C16" s="19">
         <v>5305</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="24" t="s">
+      <c r="A17" s="19" t="s">
         <v>14</v>
       </c>
       <c r="B17">
         <v>2018</v>
       </c>
-      <c r="C17" s="24">
+      <c r="C17" s="19">
         <v>2966</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="24" t="s">
+      <c r="A18" s="19" t="s">
         <v>15</v>
       </c>
       <c r="B18">
         <v>2018</v>
       </c>
-      <c r="C18" s="24">
+      <c r="C18" s="19">
         <v>304</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="24" t="s">
+      <c r="A19" s="19" t="s">
         <v>16</v>
       </c>
       <c r="B19">
         <v>2018</v>
       </c>
-      <c r="C19" s="24">
+      <c r="C19" s="19">
         <v>66</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="24" t="s">
+      <c r="A20" s="19" t="s">
         <v>11</v>
       </c>
       <c r="B20">
         <v>2019</v>
       </c>
-      <c r="C20" s="24">
+      <c r="C20" s="19">
         <v>87522</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="24" t="s">
+      <c r="A21" s="19" t="s">
         <v>12</v>
       </c>
       <c r="B21">
         <v>2019</v>
       </c>
-      <c r="C21" s="24">
+      <c r="C21" s="19">
         <v>17628</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="24" t="s">
+      <c r="A22" s="19" t="s">
         <v>13</v>
       </c>
       <c r="B22">
         <v>2019</v>
       </c>
-      <c r="C22" s="24">
+      <c r="C22" s="19">
         <v>6086</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" s="24" t="s">
+      <c r="A23" s="19" t="s">
         <v>14</v>
       </c>
       <c r="B23">
         <v>2019</v>
       </c>
-      <c r="C23" s="24">
+      <c r="C23" s="19">
         <v>3900</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" s="24" t="s">
+      <c r="A24" s="19" t="s">
         <v>15</v>
       </c>
       <c r="B24">
         <v>2019</v>
       </c>
-      <c r="C24" s="24">
+      <c r="C24" s="19">
         <v>398</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" s="24" t="s">
+      <c r="A25" s="19" t="s">
         <v>16</v>
       </c>
       <c r="B25">
         <v>2019</v>
       </c>
-      <c r="C25" s="24">
+      <c r="C25" s="19">
         <v>69</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" s="24" t="s">
+      <c r="A26" s="19" t="s">
         <v>11</v>
       </c>
       <c r="B26">
         <v>2020</v>
       </c>
-      <c r="C26" s="24">
+      <c r="C26" s="19">
         <v>72918</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" s="24" t="s">
+      <c r="A27" s="19" t="s">
         <v>12</v>
       </c>
       <c r="B27">
         <v>2020</v>
       </c>
-      <c r="C27" s="24">
+      <c r="C27" s="19">
         <v>17558</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28" s="24" t="s">
+      <c r="A28" s="19" t="s">
         <v>13</v>
       </c>
       <c r="B28">
         <v>2020</v>
       </c>
-      <c r="C28" s="24">
+      <c r="C28" s="19">
         <v>4423</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29" s="24" t="s">
+      <c r="A29" s="19" t="s">
         <v>14</v>
       </c>
       <c r="B29">
         <v>2020</v>
       </c>
-      <c r="C29" s="24">
+      <c r="C29" s="19">
         <v>4134</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30" s="24" t="s">
+      <c r="A30" s="19" t="s">
         <v>15</v>
       </c>
       <c r="B30">
         <v>2020</v>
       </c>
-      <c r="C30" s="24">
+      <c r="C30" s="19">
         <v>154</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A31" s="24" t="s">
+      <c r="A31" s="19" t="s">
         <v>16</v>
       </c>
       <c r="B31">
         <v>2020</v>
       </c>
-      <c r="C31" s="24">
+      <c r="C31" s="19">
         <v>181</v>
       </c>
     </row>
@@ -4231,242 +4143,242 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="27.7109375" customWidth="1"/>
-    <col min="3" max="3" width="9.140625" style="27"/>
+    <col min="3" max="3" width="9.140625" style="22"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="B1" s="26" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="26" t="s">
+      <c r="B1" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="21" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="24" t="s">
+      <c r="A2" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="B2" s="26">
+      <c r="B2" s="21">
         <v>2016</v>
       </c>
-      <c r="C2" s="28">
+      <c r="C2" s="23">
         <v>120</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="24" t="s">
+      <c r="A3" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="B3" s="26">
+      <c r="B3" s="21">
         <v>2016</v>
       </c>
-      <c r="C3" s="28">
+      <c r="C3" s="23">
         <v>61</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="30" t="s">
+      <c r="A4" s="25" t="s">
         <v>20</v>
       </c>
-      <c r="B4" s="26">
+      <c r="B4" s="21">
         <v>2016</v>
       </c>
-      <c r="C4" s="28">
+      <c r="C4" s="23">
         <v>285</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="24" t="s">
+      <c r="A5" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="B5" s="26">
+      <c r="B5" s="21">
         <v>2016</v>
       </c>
-      <c r="C5" s="28">
+      <c r="C5" s="23">
         <v>2909</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="24" t="s">
+      <c r="A6" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="B6" s="26">
+      <c r="B6" s="21">
         <v>2017</v>
       </c>
-      <c r="C6" s="28">
+      <c r="C6" s="23">
         <v>98</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="24" t="s">
+      <c r="A7" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="B7" s="26">
+      <c r="B7" s="21">
         <v>2017</v>
       </c>
-      <c r="C7" s="28">
+      <c r="C7" s="23">
         <v>35</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="30" t="s">
+      <c r="A8" s="25" t="s">
         <v>20</v>
       </c>
-      <c r="B8" s="26">
+      <c r="B8" s="21">
         <v>2017</v>
       </c>
-      <c r="C8" s="28">
+      <c r="C8" s="23">
         <v>275</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="24" t="s">
+      <c r="A9" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="B9" s="26">
+      <c r="B9" s="21">
         <v>2017</v>
       </c>
-      <c r="C9" s="28">
+      <c r="C9" s="23">
         <v>1663</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="24" t="s">
+      <c r="A10" s="19" t="s">
         <v>18</v>
       </c>
       <c r="B10" s="1">
         <v>2018</v>
       </c>
-      <c r="C10" s="28">
+      <c r="C10" s="23">
         <v>305</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="24" t="s">
+      <c r="A11" s="19" t="s">
         <v>19</v>
       </c>
       <c r="B11" s="1">
         <v>2018</v>
       </c>
-      <c r="C11" s="28">
+      <c r="C11" s="23">
         <v>57</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="30" t="s">
+      <c r="A12" s="25" t="s">
         <v>20</v>
       </c>
       <c r="B12" s="1">
         <v>2018</v>
       </c>
-      <c r="C12" s="28">
+      <c r="C12" s="23">
         <v>310</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="24" t="s">
+      <c r="A13" s="19" t="s">
         <v>21</v>
       </c>
       <c r="B13" s="1">
         <v>2018</v>
       </c>
-      <c r="C13" s="28">
+      <c r="C13" s="23">
         <v>2570</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="24" t="s">
+      <c r="A14" s="19" t="s">
         <v>18</v>
       </c>
       <c r="B14" s="1">
         <v>2019</v>
       </c>
-      <c r="C14" s="28">
+      <c r="C14" s="23">
         <v>424</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="24" t="s">
+      <c r="A15" s="19" t="s">
         <v>19</v>
       </c>
       <c r="B15" s="1">
         <v>2019</v>
       </c>
-      <c r="C15" s="28">
+      <c r="C15" s="23">
         <v>51</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="30" t="s">
+      <c r="A16" s="25" t="s">
         <v>20</v>
       </c>
       <c r="B16" s="1">
         <v>2019</v>
       </c>
-      <c r="C16" s="28">
+      <c r="C16" s="23">
         <v>447</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="24" t="s">
+      <c r="A17" s="19" t="s">
         <v>21</v>
       </c>
       <c r="B17" s="1">
         <v>2019</v>
       </c>
-      <c r="C17" s="28">
+      <c r="C17" s="23">
         <v>3037</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="24" t="s">
+      <c r="A18" s="19" t="s">
         <v>18</v>
       </c>
       <c r="B18" s="1">
         <v>2020</v>
       </c>
-      <c r="C18" s="28">
+      <c r="C18" s="23">
         <v>741</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="24" t="s">
+      <c r="A19" s="19" t="s">
         <v>19</v>
       </c>
       <c r="B19" s="1">
         <v>2020</v>
       </c>
-      <c r="C19" s="28">
+      <c r="C19" s="23">
         <v>78</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="30" t="s">
+      <c r="A20" s="25" t="s">
         <v>20</v>
       </c>
       <c r="B20" s="1">
         <v>2020</v>
       </c>
-      <c r="C20" s="28">
+      <c r="C20" s="23">
         <v>1221</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="24" t="s">
+      <c r="A21" s="19" t="s">
         <v>21</v>
       </c>
       <c r="B21" s="1">
         <v>2020</v>
       </c>
-      <c r="C21" s="28">
+      <c r="C21" s="23">
         <v>3838</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C22" s="26"/>
+      <c r="C22" s="21"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4487,255 +4399,255 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="25" t="s">
+      <c r="A1" s="20" t="s">
         <v>36</v>
       </c>
-      <c r="B1" s="26" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="26" t="s">
+      <c r="B1" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="21" t="s">
         <v>10</v>
       </c>
-      <c r="D1" s="29"/>
-      <c r="E1" s="29"/>
-      <c r="F1" s="29"/>
-      <c r="G1" s="29"/>
-      <c r="H1" s="29"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
+      <c r="G1" s="24"/>
+      <c r="H1" s="24"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="25" t="s">
+      <c r="A2" s="20" t="s">
         <v>37</v>
       </c>
       <c r="B2" s="1">
         <v>2016</v>
       </c>
-      <c r="C2" s="28">
+      <c r="C2" s="23">
         <v>6315</v>
       </c>
-      <c r="D2" s="25"/>
-      <c r="E2" s="25"/>
-      <c r="H2" s="25"/>
+      <c r="D2" s="20"/>
+      <c r="E2" s="20"/>
+      <c r="H2" s="20"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="25" t="s">
+      <c r="A3" s="20" t="s">
         <v>38</v>
       </c>
       <c r="B3" s="1">
         <v>2016</v>
       </c>
-      <c r="C3" s="28">
+      <c r="C3" s="23">
         <v>4787</v>
       </c>
-      <c r="D3" s="25"/>
-      <c r="E3" s="25"/>
-      <c r="H3" s="25"/>
+      <c r="D3" s="20"/>
+      <c r="E3" s="20"/>
+      <c r="H3" s="20"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="25" t="s">
+      <c r="A4" s="20" t="s">
         <v>39</v>
       </c>
       <c r="B4" s="1">
         <v>2016</v>
       </c>
-      <c r="C4" s="28">
+      <c r="C4" s="23">
         <v>3375</v>
       </c>
-      <c r="D4" s="25"/>
-      <c r="E4" s="25"/>
-      <c r="H4" s="25"/>
+      <c r="D4" s="20"/>
+      <c r="E4" s="20"/>
+      <c r="H4" s="20"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="25" t="s">
+      <c r="A5" s="20" t="s">
         <v>40</v>
       </c>
       <c r="B5" s="1">
         <v>2016</v>
       </c>
-      <c r="C5" s="28">
+      <c r="C5" s="23">
         <v>55</v>
       </c>
-      <c r="D5" s="25"/>
-      <c r="E5" s="25"/>
-      <c r="H5" s="25"/>
+      <c r="D5" s="20"/>
+      <c r="E5" s="20"/>
+      <c r="H5" s="20"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="25" t="s">
+      <c r="A6" s="20" t="s">
         <v>37</v>
       </c>
       <c r="B6" s="1">
         <v>2017</v>
       </c>
-      <c r="C6" s="28">
+      <c r="C6" s="23">
         <v>6456</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="25" t="s">
+      <c r="A7" s="20" t="s">
         <v>38</v>
       </c>
       <c r="B7" s="1">
         <v>2017</v>
       </c>
-      <c r="C7" s="28">
+      <c r="C7" s="23">
         <v>4320</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="25" t="s">
+      <c r="A8" s="20" t="s">
         <v>39</v>
       </c>
       <c r="B8" s="1">
         <v>2017</v>
       </c>
-      <c r="C8" s="28">
+      <c r="C8" s="23">
         <v>2070</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="25" t="s">
+      <c r="A9" s="20" t="s">
         <v>40</v>
       </c>
       <c r="B9" s="1">
         <v>2017</v>
       </c>
-      <c r="C9" s="28">
+      <c r="C9" s="23">
         <v>50</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="25" t="s">
+      <c r="A10" s="20" t="s">
         <v>37</v>
       </c>
-      <c r="B10" s="26">
+      <c r="B10" s="21">
         <v>2018</v>
       </c>
-      <c r="C10" s="28">
+      <c r="C10" s="23">
         <v>7096</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="25" t="s">
+      <c r="A11" s="20" t="s">
         <v>38</v>
       </c>
-      <c r="B11" s="26">
+      <c r="B11" s="21">
         <v>2018</v>
       </c>
-      <c r="C11" s="28">
+      <c r="C11" s="23">
         <v>4153</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="25" t="s">
+      <c r="A12" s="20" t="s">
         <v>39</v>
       </c>
-      <c r="B12" s="26">
+      <c r="B12" s="21">
         <v>2018</v>
       </c>
-      <c r="C12" s="28">
+      <c r="C12" s="23">
         <v>3242</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="25" t="s">
+      <c r="A13" s="20" t="s">
         <v>40</v>
       </c>
-      <c r="B13" s="26">
+      <c r="B13" s="21">
         <v>2018</v>
       </c>
-      <c r="C13" s="28">
+      <c r="C13" s="23">
         <v>44</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="25" t="s">
+      <c r="A14" s="20" t="s">
         <v>37</v>
       </c>
-      <c r="B14" s="26">
+      <c r="B14" s="21">
         <v>2019</v>
       </c>
-      <c r="C14" s="28">
+      <c r="C14" s="23">
         <v>7515</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="25" t="s">
+      <c r="A15" s="20" t="s">
         <v>38</v>
       </c>
-      <c r="B15" s="26">
+      <c r="B15" s="21">
         <v>2019</v>
       </c>
-      <c r="C15" s="28">
+      <c r="C15" s="23">
         <v>6221</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="25" t="s">
+      <c r="A16" s="20" t="s">
         <v>39</v>
       </c>
-      <c r="B16" s="26">
+      <c r="B16" s="21">
         <v>2019</v>
       </c>
-      <c r="C16" s="28">
+      <c r="C16" s="23">
         <v>3916</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="25" t="s">
+      <c r="A17" s="20" t="s">
         <v>40</v>
       </c>
-      <c r="B17" s="26">
+      <c r="B17" s="21">
         <v>2019</v>
       </c>
-      <c r="C17" s="28">
+      <c r="C17" s="23">
         <v>43</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="25" t="s">
+      <c r="A18" s="20" t="s">
         <v>37</v>
       </c>
       <c r="B18" s="1">
         <v>2020</v>
       </c>
-      <c r="C18" s="28">
+      <c r="C18" s="23">
         <v>6798</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="25" t="s">
+      <c r="A19" s="20" t="s">
         <v>38</v>
       </c>
       <c r="B19" s="1">
         <v>2020</v>
       </c>
-      <c r="C19" s="28">
+      <c r="C19" s="23">
         <v>5532</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="25" t="s">
+      <c r="A20" s="20" t="s">
         <v>39</v>
       </c>
       <c r="B20" s="1">
         <v>2020</v>
       </c>
-      <c r="C20" s="28">
+      <c r="C20" s="23">
         <v>51</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="25" t="s">
+      <c r="A21" s="20" t="s">
         <v>40</v>
       </c>
       <c r="B21" s="1">
         <v>2020</v>
       </c>
-      <c r="C21" s="28">
+      <c r="C21" s="23">
         <v>5827</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C22" s="26"/>
+      <c r="C22" s="21"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4744,10 +4656,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B7353AB-3A1D-4F1C-8F3A-DB45EED24601}">
-  <dimension ref="A1:C12"/>
+  <dimension ref="A1:C13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4770,135 +4682,147 @@
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="36">
+      <c r="A2" s="30">
         <v>2010</v>
       </c>
-      <c r="B2" s="37">
+      <c r="B2" s="31">
         <v>4.8000000000000001E-2</v>
       </c>
-      <c r="C2" s="37">
+      <c r="C2" s="31">
         <f>1-B2</f>
         <v>0.95199999999999996</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="36">
+      <c r="A3" s="30">
         <v>2011</v>
       </c>
-      <c r="B3" s="37">
+      <c r="B3" s="31">
         <v>4.2000000000000003E-2</v>
       </c>
-      <c r="C3" s="37">
-        <f t="shared" ref="C3:C12" si="0">1-B3</f>
+      <c r="C3" s="31">
+        <f t="shared" ref="C3:C13" si="0">1-B3</f>
         <v>0.95799999999999996</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="36">
+      <c r="A4" s="30">
         <v>2012</v>
       </c>
-      <c r="B4" s="37">
+      <c r="B4" s="31">
         <v>0.03</v>
       </c>
-      <c r="C4" s="37">
+      <c r="C4" s="31">
         <f t="shared" si="0"/>
         <v>0.97</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="36">
+      <c r="A5" s="30">
         <v>2013</v>
       </c>
-      <c r="B5" s="37">
+      <c r="B5" s="31">
         <v>2.5999999999999999E-2</v>
       </c>
-      <c r="C5" s="37">
+      <c r="C5" s="31">
         <f t="shared" si="0"/>
         <v>0.97399999999999998</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="36">
+      <c r="A6" s="30">
         <v>2014</v>
       </c>
-      <c r="B6" s="37">
+      <c r="B6" s="31">
         <v>2.7E-2</v>
       </c>
-      <c r="C6" s="37">
+      <c r="C6" s="31">
         <f t="shared" si="0"/>
         <v>0.97299999999999998</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="36">
+      <c r="A7" s="30">
         <v>2015</v>
       </c>
-      <c r="B7" s="37">
+      <c r="B7" s="31">
         <v>3.7999999999999999E-2</v>
       </c>
-      <c r="C7" s="37">
+      <c r="C7" s="31">
         <f t="shared" si="0"/>
         <v>0.96199999999999997</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="36">
+      <c r="A8" s="30">
         <v>2016</v>
       </c>
-      <c r="B8" s="37">
+      <c r="B8" s="31">
         <v>2.3E-2</v>
       </c>
-      <c r="C8" s="37">
+      <c r="C8" s="31">
         <f t="shared" si="0"/>
         <v>0.97699999999999998</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="36">
+      <c r="A9" s="30">
         <v>2017</v>
       </c>
-      <c r="B9" s="37">
+      <c r="B9" s="31">
         <v>2.4E-2</v>
       </c>
-      <c r="C9" s="37">
+      <c r="C9" s="31">
         <f t="shared" si="0"/>
         <v>0.97599999999999998</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="36">
+      <c r="A10" s="30">
         <v>2018</v>
       </c>
-      <c r="B10" s="37">
+      <c r="B10" s="31">
         <v>2.9000000000000001E-2</v>
       </c>
-      <c r="C10" s="37">
+      <c r="C10" s="31">
         <f t="shared" si="0"/>
         <v>0.97099999999999997</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="36">
+      <c r="A11" s="30">
         <v>2019</v>
       </c>
-      <c r="B11" s="37">
+      <c r="B11" s="31">
         <v>3.7999999999999999E-2</v>
       </c>
-      <c r="C11" s="37">
+      <c r="C11" s="31">
         <f t="shared" si="0"/>
         <v>0.96199999999999997</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="36">
+      <c r="A12" s="30">
         <v>2020</v>
       </c>
-      <c r="B12" s="37">
+      <c r="B12" s="31">
         <v>5.1999999999999998E-2</v>
       </c>
-      <c r="C12" s="37">
+      <c r="C12" s="31">
         <f t="shared" si="0"/>
         <v>0.94799999999999995</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="1">
+        <v>2021</v>
+      </c>
+      <c r="B13" s="31">
+        <v>3.5000000000000003E-2</v>
+      </c>
+      <c r="C13" s="31">
+        <f t="shared" si="0"/>
+        <v>0.96499999999999997</v>
       </c>
     </row>
   </sheetData>
@@ -4928,19 +4852,19 @@
       <c r="A2" s="1">
         <v>2016</v>
       </c>
-      <c r="B2" s="20">
+      <c r="B2" s="15">
         <v>0.15</v>
       </c>
-      <c r="C2" s="7"/>
-      <c r="D2" s="7"/>
-      <c r="E2" s="7"/>
-      <c r="F2" s="5"/>
+      <c r="C2" s="6"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6"/>
+      <c r="F2" s="4"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>2017</v>
       </c>
-      <c r="B3" s="20">
+      <c r="B3" s="15">
         <v>0.12</v>
       </c>
     </row>
@@ -4948,7 +4872,7 @@
       <c r="A4" s="1">
         <v>2018</v>
       </c>
-      <c r="B4" s="20">
+      <c r="B4" s="15">
         <v>0.15</v>
       </c>
     </row>
@@ -4956,7 +4880,7 @@
       <c r="A5" s="1">
         <v>2019</v>
       </c>
-      <c r="B5" s="20">
+      <c r="B5" s="15">
         <v>0.17</v>
       </c>
     </row>
@@ -4964,7 +4888,7 @@
       <c r="A6" s="1">
         <v>2020</v>
       </c>
-      <c r="B6" s="20">
+      <c r="B6" s="15">
         <v>0.20280000000000001</v>
       </c>
     </row>
@@ -5003,16 +4927,16 @@
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="E1" s="5" t="s">
         <v>47</v>
       </c>
       <c r="F1" t="s">
@@ -5032,28 +4956,28 @@
       <c r="A2">
         <v>2016</v>
       </c>
-      <c r="B2" s="6">
+      <c r="B2" s="5">
         <v>90331</v>
       </c>
-      <c r="C2" s="6">
+      <c r="C2" s="5">
         <v>85961</v>
       </c>
-      <c r="D2" s="21">
+      <c r="D2" s="16">
         <v>0.95199999999999996</v>
       </c>
-      <c r="E2" s="6">
+      <c r="E2" s="5">
         <v>57995</v>
       </c>
-      <c r="F2" s="6">
+      <c r="F2" s="5">
         <v>27</v>
       </c>
-      <c r="G2" s="6">
+      <c r="G2" s="5">
         <v>30</v>
       </c>
-      <c r="H2" s="6">
+      <c r="H2" s="5">
         <v>28</v>
       </c>
-      <c r="I2" s="6">
+      <c r="I2" s="5">
         <v>9</v>
       </c>
     </row>
@@ -5061,28 +4985,28 @@
       <c r="A3">
         <v>2017</v>
       </c>
-      <c r="B3" s="6">
+      <c r="B3" s="5">
         <v>103650</v>
       </c>
-      <c r="C3" s="6">
+      <c r="C3" s="5">
         <v>115402</v>
       </c>
-      <c r="D3" s="21">
+      <c r="D3" s="16">
         <v>1.133</v>
       </c>
-      <c r="E3" s="6">
+      <c r="E3" s="5">
         <v>45425</v>
       </c>
-      <c r="F3" s="6">
+      <c r="F3" s="5">
         <v>39</v>
       </c>
-      <c r="G3" s="6">
+      <c r="G3" s="5">
         <v>12</v>
       </c>
-      <c r="H3" s="6">
+      <c r="H3" s="5">
         <v>38</v>
       </c>
-      <c r="I3" s="6">
+      <c r="I3" s="5">
         <v>9</v>
       </c>
     </row>
@@ -5090,28 +5014,28 @@
       <c r="A4">
         <v>2018</v>
       </c>
-      <c r="B4" s="6">
+      <c r="B4" s="5">
         <v>101497</v>
       </c>
-      <c r="C4" s="6">
+      <c r="C4" s="5">
         <v>106452</v>
       </c>
-      <c r="D4" s="21">
+      <c r="D4" s="16">
         <v>1.0489999999999999</v>
       </c>
-      <c r="E4" s="6">
+      <c r="E4" s="5">
         <v>38975</v>
       </c>
-      <c r="F4" s="6">
+      <c r="F4" s="5">
         <v>32</v>
       </c>
-      <c r="G4" s="6">
+      <c r="G4" s="5">
         <v>11</v>
       </c>
-      <c r="H4" s="6">
+      <c r="H4" s="5">
         <v>23</v>
       </c>
-      <c r="I4" s="6">
+      <c r="I4" s="5">
         <v>4</v>
       </c>
     </row>
@@ -5119,28 +5043,28 @@
       <c r="A5">
         <v>2019</v>
       </c>
-      <c r="B5" s="6">
+      <c r="B5" s="5">
         <v>93197</v>
       </c>
-      <c r="C5" s="6">
+      <c r="C5" s="5">
         <v>96896</v>
       </c>
-      <c r="D5" s="21">
+      <c r="D5" s="16">
         <v>1.0389999999999999</v>
       </c>
-      <c r="E5" s="6">
+      <c r="E5" s="5">
         <v>31279</v>
       </c>
-      <c r="F5" s="6">
+      <c r="F5" s="5">
         <v>41</v>
       </c>
-      <c r="G5" s="6">
+      <c r="G5" s="5">
         <v>10</v>
       </c>
-      <c r="H5" s="6">
+      <c r="H5" s="5">
         <v>24</v>
       </c>
-      <c r="I5" s="6">
+      <c r="I5" s="5">
         <v>7</v>
       </c>
     </row>
@@ -5148,85 +5072,85 @@
       <c r="A6">
         <v>2020</v>
       </c>
-      <c r="B6" s="6">
+      <c r="B6" s="5">
         <v>75137</v>
       </c>
-      <c r="C6" s="6">
+      <c r="C6" s="5">
         <v>78433</v>
       </c>
-      <c r="D6" s="21">
+      <c r="D6" s="16">
         <f>C6/B6</f>
         <v>1.0438665371255174</v>
       </c>
-      <c r="E6" s="6">
+      <c r="E6" s="5">
         <v>26256</v>
       </c>
-      <c r="F6" s="6">
+      <c r="F6" s="5">
         <v>30</v>
       </c>
-      <c r="G6" s="6">
+      <c r="G6" s="5">
         <v>22</v>
       </c>
-      <c r="H6" s="6">
+      <c r="H6" s="5">
         <v>125</v>
       </c>
-      <c r="I6" s="6">
+      <c r="I6" s="5">
         <v>9</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="G9" s="6"/>
-      <c r="H9" s="6"/>
-      <c r="I9" s="6"/>
-      <c r="J9" s="6"/>
-      <c r="K9" s="6"/>
+      <c r="G9" s="5"/>
+      <c r="H9" s="5"/>
+      <c r="I9" s="5"/>
+      <c r="J9" s="5"/>
+      <c r="K9" s="5"/>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="J10" s="6"/>
-      <c r="K10" s="6"/>
-      <c r="L10" s="6"/>
-      <c r="M10" s="6"/>
-      <c r="N10" s="6"/>
+      <c r="J10" s="5"/>
+      <c r="K10" s="5"/>
+      <c r="L10" s="5"/>
+      <c r="M10" s="5"/>
+      <c r="N10" s="5"/>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="G11" s="6"/>
-      <c r="J11" s="6"/>
-      <c r="K11" s="6"/>
-      <c r="L11" s="6"/>
-      <c r="M11" s="6"/>
-      <c r="N11" s="6"/>
+      <c r="G11" s="5"/>
+      <c r="J11" s="5"/>
+      <c r="K11" s="5"/>
+      <c r="L11" s="5"/>
+      <c r="M11" s="5"/>
+      <c r="N11" s="5"/>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="G12" s="6"/>
+      <c r="G12" s="5"/>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="G13" s="6"/>
+      <c r="G13" s="5"/>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="G14" s="6"/>
+      <c r="G14" s="5"/>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="G15" s="6"/>
+      <c r="G15" s="5"/>
     </row>
     <row r="19" spans="7:9" x14ac:dyDescent="0.25">
-      <c r="G19" s="6"/>
-      <c r="H19" s="6"/>
-      <c r="I19" s="6"/>
+      <c r="G19" s="5"/>
+      <c r="H19" s="5"/>
+      <c r="I19" s="5"/>
     </row>
     <row r="21" spans="7:9" x14ac:dyDescent="0.25">
-      <c r="G21" s="6"/>
+      <c r="G21" s="5"/>
     </row>
     <row r="22" spans="7:9" x14ac:dyDescent="0.25">
-      <c r="G22" s="6"/>
+      <c r="G22" s="5"/>
     </row>
     <row r="23" spans="7:9" x14ac:dyDescent="0.25">
-      <c r="G23" s="6"/>
+      <c r="G23" s="5"/>
     </row>
     <row r="24" spans="7:9" x14ac:dyDescent="0.25">
-      <c r="G24" s="6"/>
+      <c r="G24" s="5"/>
     </row>
     <row r="25" spans="7:9" x14ac:dyDescent="0.25">
-      <c r="G25" s="6"/>
+      <c r="G25" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Alterações realizadas até 10/12/2021.
</commit_message>
<xml_diff>
--- a/dados/relatorio_historico.xlsx
+++ b/dados/relatorio_historico.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24701"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\arian\Desktop\R_STF\Relatorio_R\Git\Code-Relatorio\dados\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{349B585B-AAD3-430E-90CD-BCAEC1E7D775}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{990D1F03-3995-4D70-9CD2-015128EFE29D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11160" firstSheet="1" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="9" hidden="1">recebidos_classe!$A$1:$G$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="10" hidden="1">'recebidos_classe (2)'!$A$1:$G$1</definedName>
   </definedNames>
-  <calcPr calcId="191028" refMode="R1C1" iterateCount="0" calcOnSave="0" concurrentCalc="0"/>
+  <calcPr calcId="191028" iterateCount="1" calcOnSave="0" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -146,7 +146,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="289" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="105">
   <si>
     <t>ano</t>
   </si>
@@ -459,6 +459,12 @@
   </si>
   <si>
     <t>STA</t>
+  </si>
+  <si>
+    <t>are_prov</t>
+  </si>
+  <si>
+    <t>re_prov</t>
   </si>
 </sst>
 </file>
@@ -700,7 +706,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="65">
+  <cellXfs count="66">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -878,6 +884,7 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4656,10 +4663,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B7353AB-3A1D-4F1C-8F3A-DB45EED24601}">
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="L13" sqref="L13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4670,7 +4677,7 @@
     <col min="4" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -4680,8 +4687,14 @@
       <c r="C1" s="1" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D1" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="30">
         <v>2010</v>
       </c>
@@ -4692,8 +4705,12 @@
         <f>1-B2</f>
         <v>0.95199999999999996</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D2" s="31"/>
+      <c r="E2" s="65">
+        <v>0.1657248298927459</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="30">
         <v>2011</v>
       </c>
@@ -4704,8 +4721,14 @@
         <f t="shared" ref="C3:C13" si="0">1-B3</f>
         <v>0.95799999999999996</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D3" s="31">
+        <v>1.0590228748940981E-2</v>
+      </c>
+      <c r="E3" s="65">
+        <v>0.14890586559627089</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="30">
         <v>2012</v>
       </c>
@@ -4716,8 +4739,14 @@
         <f t="shared" si="0"/>
         <v>0.97</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D4" s="31">
+        <v>1.243592600846891E-2</v>
+      </c>
+      <c r="E4" s="65">
+        <v>0.1237701692247147</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="30">
         <v>2013</v>
       </c>
@@ -4728,8 +4757,14 @@
         <f t="shared" si="0"/>
         <v>0.97399999999999998</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D5" s="31">
+        <v>9.0879931572757401E-3</v>
+      </c>
+      <c r="E5" s="65">
+        <v>9.4643503438291712E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="30">
         <v>2014</v>
       </c>
@@ -4740,8 +4775,14 @@
         <f t="shared" si="0"/>
         <v>0.97299999999999998</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D6" s="31">
+        <v>9.1809470237258165E-3</v>
+      </c>
+      <c r="E6" s="65">
+        <v>0.14798514647228719</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="30">
         <v>2015</v>
       </c>
@@ -4752,8 +4793,14 @@
         <f t="shared" si="0"/>
         <v>0.96199999999999997</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D7" s="31">
+        <v>9.0755082284607932E-3</v>
+      </c>
+      <c r="E7" s="65">
+        <v>0.21354916067146279</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="30">
         <v>2016</v>
       </c>
@@ -4764,8 +4811,14 @@
         <f t="shared" si="0"/>
         <v>0.97699999999999998</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D8" s="31">
+        <v>7.3168287060238557E-3</v>
+      </c>
+      <c r="E8" s="65">
+        <v>0.13724928366762179</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="30">
         <v>2017</v>
       </c>
@@ -4776,8 +4829,14 @@
         <f t="shared" si="0"/>
         <v>0.97599999999999998</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D9" s="31">
+        <v>8.2126553524233883E-3</v>
+      </c>
+      <c r="E9" s="65">
+        <v>0.12197496522948539</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="30">
         <v>2018</v>
       </c>
@@ -4788,8 +4847,14 @@
         <f t="shared" si="0"/>
         <v>0.97099999999999997</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D10" s="31">
+        <v>6.8021830261804951E-3</v>
+      </c>
+      <c r="E10" s="65">
+        <v>0.15828939660222621</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="30">
         <v>2019</v>
       </c>
@@ -4800,8 +4865,14 @@
         <f t="shared" si="0"/>
         <v>0.96199999999999997</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D11" s="31">
+        <v>1.0522700306001369E-2</v>
+      </c>
+      <c r="E11" s="65">
+        <v>0.16755741730463669</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="30">
         <v>2020</v>
       </c>
@@ -4812,8 +4883,14 @@
         <f t="shared" si="0"/>
         <v>0.94799999999999995</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D12" s="31">
+        <v>1.211535929063693E-2</v>
+      </c>
+      <c r="E12" s="65">
+        <v>0.22150497971228331</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>2021</v>
       </c>
@@ -4823,6 +4900,12 @@
       <c r="C13" s="31">
         <f t="shared" si="0"/>
         <v>0.96499999999999997</v>
+      </c>
+      <c r="D13" s="31">
+        <v>1.252696200431392E-2</v>
+      </c>
+      <c r="E13" s="65">
+        <v>0.1588950276243094</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Tabela de provimento atualizada com ARE e RE (2021).
</commit_message>
<xml_diff>
--- a/dados/relatorio_historico.xlsx
+++ b/dados/relatorio_historico.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\arian\Desktop\R_STF\Relatorio_R\Git\Code-Relatorio\dados\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{990D1F03-3995-4D70-9CD2-015128EFE29D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9007CFAD-09B4-4ACC-80D3-F5FE8D5E78F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11160" firstSheet="1" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="1" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="acervo" sheetId="1" r:id="rId1"/>
@@ -4666,7 +4666,7 @@
   <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L13" sqref="L13"/>
+      <selection activeCell="N12" sqref="N12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Commitando parte de RG
</commit_message>
<xml_diff>
--- a/dados/relatorio_historico.xlsx
+++ b/dados/relatorio_historico.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\arian\Desktop\R_STF\Relatorio_R\Git\Code-Relatorio\dados\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Euler.Alencar\Documents\05. Projetos_r\github_projects\Code-Relatorio\dados\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{349B585B-AAD3-430E-90CD-BCAEC1E7D775}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90423173-1D1C-4793-93D2-04B7AFA4382E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11160" firstSheet="1" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6195" yWindow="2595" windowWidth="21600" windowHeight="11385" firstSheet="5" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="acervo" sheetId="1" r:id="rId1"/>
@@ -23,11 +23,12 @@
     <sheet name="recorribilidade" sheetId="11" r:id="rId8"/>
     <sheet name="produtividade" sheetId="12" r:id="rId9"/>
     <sheet name="recebidos_classe" sheetId="3" r:id="rId10"/>
-    <sheet name="recebidos_classe (2)" sheetId="17" state="hidden" r:id="rId11"/>
+    <sheet name="rg" sheetId="18" r:id="rId11"/>
+    <sheet name="recebidos_classe (2)" sheetId="17" state="hidden" r:id="rId12"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="9" hidden="1">recebidos_classe!$A$1:$G$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="10" hidden="1">'recebidos_classe (2)'!$A$1:$G$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="11" hidden="1">'recebidos_classe (2)'!$A$1:$G$1</definedName>
   </definedNames>
   <calcPr calcId="191028" refMode="R1C1" iterateCount="0" calcOnSave="0" concurrentCalc="0"/>
   <extLst>
@@ -37,7 +38,6 @@
         <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -146,7 +146,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="289" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="294" uniqueCount="108">
   <si>
     <t>ano</t>
   </si>
@@ -459,6 +459,21 @@
   </si>
   <si>
     <t>STA</t>
+  </si>
+  <si>
+    <t>RG</t>
+  </si>
+  <si>
+    <t>Repercussão Geral Reconhecida</t>
+  </si>
+  <si>
+    <t>Repercussão Geral Negada</t>
+  </si>
+  <si>
+    <t>Mérito Julgado</t>
+  </si>
+  <si>
+    <t>Reafirmação de Jurisprudência</t>
   </si>
 </sst>
 </file>
@@ -468,7 +483,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0%"/>
   </numFmts>
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -529,6 +544,13 @@
       <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <charset val="1"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -700,7 +722,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="65">
+  <cellXfs count="66">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -877,6 +899,9 @@
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment readingOrder="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2335,6 +2360,124 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8F46296-CF02-4BA5-9E80-7EE57AE1BA24}">
+  <dimension ref="A1:F5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="29.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="65" t="s">
+        <v>103</v>
+      </c>
+      <c r="B1" s="65">
+        <v>2016</v>
+      </c>
+      <c r="C1" s="65">
+        <v>2017</v>
+      </c>
+      <c r="D1" s="65">
+        <v>2018</v>
+      </c>
+      <c r="E1" s="65">
+        <v>2019</v>
+      </c>
+      <c r="F1" s="65">
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="65" t="s">
+        <v>104</v>
+      </c>
+      <c r="B2" s="65">
+        <v>27</v>
+      </c>
+      <c r="C2" s="65">
+        <v>39</v>
+      </c>
+      <c r="D2" s="65">
+        <v>32</v>
+      </c>
+      <c r="E2" s="65">
+        <v>41</v>
+      </c>
+      <c r="F2" s="65">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="65" t="s">
+        <v>105</v>
+      </c>
+      <c r="B3" s="65">
+        <v>30</v>
+      </c>
+      <c r="C3" s="65">
+        <v>12</v>
+      </c>
+      <c r="D3" s="65">
+        <v>11</v>
+      </c>
+      <c r="E3" s="65">
+        <v>10</v>
+      </c>
+      <c r="F3" s="65">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="65" t="s">
+        <v>106</v>
+      </c>
+      <c r="B4" s="65">
+        <v>28</v>
+      </c>
+      <c r="C4" s="65">
+        <v>38</v>
+      </c>
+      <c r="D4" s="65">
+        <v>23</v>
+      </c>
+      <c r="E4" s="65">
+        <v>24</v>
+      </c>
+      <c r="F4" s="65">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="65" t="s">
+        <v>107</v>
+      </c>
+      <c r="B5" s="65">
+        <v>9</v>
+      </c>
+      <c r="C5" s="65">
+        <v>9</v>
+      </c>
+      <c r="D5" s="65">
+        <v>4</v>
+      </c>
+      <c r="E5" s="65">
+        <v>7</v>
+      </c>
+      <c r="F5" s="65">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{96DFF0C0-6C86-4302-8911-3EF065F113E7}">
   <sheetPr>
     <tabColor rgb="FFFFC000"/>
@@ -4658,7 +4801,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B7353AB-3A1D-4F1C-8F3A-DB45EED24601}">
   <dimension ref="A1:C13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Alterações realizadas até 14/12/2021. Inclusão dos gráficos: 1 - Taxa de Provimento; 2 - Decisões totais e finais.
</commit_message>
<xml_diff>
--- a/dados/relatorio_historico.xlsx
+++ b/dados/relatorio_historico.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\arian\Desktop\R_STF\Relatorio_R\Git\Code-Relatorio\dados\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9007CFAD-09B4-4ACC-80D3-F5FE8D5E78F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04D43E3D-2D18-4155-B1E5-3DC23CEFE8E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="1" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11160" firstSheet="5" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="acervo" sheetId="1" r:id="rId1"/>
@@ -4666,7 +4666,7 @@
   <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N12" sqref="N12"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4895,11 +4895,11 @@
         <v>2021</v>
       </c>
       <c r="B13" s="31">
-        <v>3.5000000000000003E-2</v>
+        <v>3.5999999999999997E-2</v>
       </c>
       <c r="C13" s="31">
         <f t="shared" si="0"/>
-        <v>0.96499999999999997</v>
+        <v>0.96399999999999997</v>
       </c>
       <c r="D13" s="31">
         <v>1.252696200431392E-2</v>

</xml_diff>

<commit_message>
Alterações realizadas até 15/12/2021. - Inclusão de RG
</commit_message>
<xml_diff>
--- a/dados/relatorio_historico.xlsx
+++ b/dados/relatorio_historico.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\arian\Desktop\R_STF\Relatorio_R\Git\Code-Relatorio\dados\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04D43E3D-2D18-4155-B1E5-3DC23CEFE8E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F41D185-A619-4746-8538-0596DFDA0374}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11160" firstSheet="5" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11160" firstSheet="5" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="acervo" sheetId="1" r:id="rId1"/>
@@ -23,13 +23,14 @@
     <sheet name="recorribilidade" sheetId="11" r:id="rId8"/>
     <sheet name="produtividade" sheetId="12" r:id="rId9"/>
     <sheet name="recebidos_classe" sheetId="3" r:id="rId10"/>
-    <sheet name="recebidos_classe (2)" sheetId="17" state="hidden" r:id="rId11"/>
+    <sheet name="rg" sheetId="18" r:id="rId11"/>
+    <sheet name="recebidos_classe (2)" sheetId="17" state="hidden" r:id="rId12"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="9" hidden="1">recebidos_classe!$A$1:$G$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="10" hidden="1">'recebidos_classe (2)'!$A$1:$G$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="11" hidden="1">'recebidos_classe (2)'!$A$1:$G$1</definedName>
   </definedNames>
-  <calcPr calcId="191028" iterateCount="1" calcOnSave="0" concurrentCalc="0"/>
+  <calcPr calcId="191028" refMode="R1C1" iterateCount="0" calcOnSave="0" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -146,7 +147,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="296" uniqueCount="110">
   <si>
     <t>ano</t>
   </si>
@@ -465,6 +466,21 @@
   </si>
   <si>
     <t>re_prov</t>
+  </si>
+  <si>
+    <t>RG</t>
+  </si>
+  <si>
+    <t>Repercussão Geral Reconhecida</t>
+  </si>
+  <si>
+    <t>Repercussão Geral Negada</t>
+  </si>
+  <si>
+    <t>Mérito Julgado</t>
+  </si>
+  <si>
+    <t>Reafirmação de Jurisprudência</t>
   </si>
 </sst>
 </file>
@@ -474,7 +490,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0%"/>
   </numFmts>
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -535,6 +551,13 @@
       <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <charset val="1"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -706,7 +729,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="66">
+  <cellXfs count="67">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -885,6 +908,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment readingOrder="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1400,12 +1426,9 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD0759C1-C855-4F22-872A-A71AC1A73C77}">
-  <sheetPr>
-    <tabColor rgb="FF00B050"/>
-  </sheetPr>
   <dimension ref="A1:G40"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="A38" sqref="A38"/>
     </sheetView>
   </sheetViews>
@@ -2342,6 +2365,124 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F05A68C-86BA-448B-BCDE-0E49F45CFCFD}">
+  <dimension ref="A1:F5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="29.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="66" t="s">
+        <v>105</v>
+      </c>
+      <c r="B1" s="66">
+        <v>2016</v>
+      </c>
+      <c r="C1" s="66">
+        <v>2017</v>
+      </c>
+      <c r="D1" s="66">
+        <v>2018</v>
+      </c>
+      <c r="E1" s="66">
+        <v>2019</v>
+      </c>
+      <c r="F1" s="66">
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="66" t="s">
+        <v>106</v>
+      </c>
+      <c r="B2" s="66">
+        <v>27</v>
+      </c>
+      <c r="C2" s="66">
+        <v>39</v>
+      </c>
+      <c r="D2" s="66">
+        <v>32</v>
+      </c>
+      <c r="E2" s="66">
+        <v>41</v>
+      </c>
+      <c r="F2" s="66">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="66" t="s">
+        <v>107</v>
+      </c>
+      <c r="B3" s="66">
+        <v>30</v>
+      </c>
+      <c r="C3" s="66">
+        <v>12</v>
+      </c>
+      <c r="D3" s="66">
+        <v>11</v>
+      </c>
+      <c r="E3" s="66">
+        <v>10</v>
+      </c>
+      <c r="F3" s="66">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="66" t="s">
+        <v>108</v>
+      </c>
+      <c r="B4" s="66">
+        <v>28</v>
+      </c>
+      <c r="C4" s="66">
+        <v>38</v>
+      </c>
+      <c r="D4" s="66">
+        <v>23</v>
+      </c>
+      <c r="E4" s="66">
+        <v>24</v>
+      </c>
+      <c r="F4" s="66">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="66" t="s">
+        <v>109</v>
+      </c>
+      <c r="B5" s="66">
+        <v>9</v>
+      </c>
+      <c r="C5" s="66">
+        <v>9</v>
+      </c>
+      <c r="D5" s="66">
+        <v>4</v>
+      </c>
+      <c r="E5" s="66">
+        <v>7</v>
+      </c>
+      <c r="F5" s="66">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{96DFF0C0-6C86-4302-8911-3EF065F113E7}">
   <sheetPr>
     <tabColor rgb="FFFFC000"/>
@@ -4665,7 +4806,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B7353AB-3A1D-4F1C-8F3A-DB45EED24601}">
   <dimension ref="A1:E13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
@@ -4991,7 +5132,7 @@
   <dimension ref="A1:N25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I17" sqref="I17"/>
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Alterações realizadas até 16/12/2021.
</commit_message>
<xml_diff>
--- a/dados/relatorio_historico.xlsx
+++ b/dados/relatorio_historico.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\arian\Desktop\R_STF\Relatorio_R\Git\Code-Relatorio\dados\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F41D185-A619-4746-8538-0596DFDA0374}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA470D17-A01F-4F65-BB09-DE11D091C803}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11160" firstSheet="5" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="13490" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="5" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="acervo" sheetId="1" r:id="rId1"/>
@@ -729,7 +729,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="67">
+  <cellXfs count="68">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -910,6 +910,9 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment readingOrder="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2368,7 +2371,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F05A68C-86BA-448B-BCDE-0E49F45CFCFD}">
   <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
@@ -4806,8 +4809,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B7353AB-3A1D-4F1C-8F3A-DB45EED24601}">
   <dimension ref="A1:E13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K12" sqref="K12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4862,7 +4865,7 @@
         <f t="shared" ref="C3:C13" si="0">1-B3</f>
         <v>0.95799999999999996</v>
       </c>
-      <c r="D3" s="31">
+      <c r="D3" s="67">
         <v>1.0590228748940981E-2</v>
       </c>
       <c r="E3" s="65">
@@ -4880,7 +4883,7 @@
         <f t="shared" si="0"/>
         <v>0.97</v>
       </c>
-      <c r="D4" s="31">
+      <c r="D4" s="67">
         <v>1.243592600846891E-2</v>
       </c>
       <c r="E4" s="65">
@@ -4898,7 +4901,7 @@
         <f t="shared" si="0"/>
         <v>0.97399999999999998</v>
       </c>
-      <c r="D5" s="31">
+      <c r="D5" s="67">
         <v>9.0879931572757401E-3</v>
       </c>
       <c r="E5" s="65">
@@ -4916,7 +4919,7 @@
         <f t="shared" si="0"/>
         <v>0.97299999999999998</v>
       </c>
-      <c r="D6" s="31">
+      <c r="D6" s="67">
         <v>9.1809470237258165E-3</v>
       </c>
       <c r="E6" s="65">
@@ -4934,7 +4937,7 @@
         <f t="shared" si="0"/>
         <v>0.96199999999999997</v>
       </c>
-      <c r="D7" s="31">
+      <c r="D7" s="67">
         <v>9.0755082284607932E-3</v>
       </c>
       <c r="E7" s="65">
@@ -4952,7 +4955,7 @@
         <f t="shared" si="0"/>
         <v>0.97699999999999998</v>
       </c>
-      <c r="D8" s="31">
+      <c r="D8" s="67">
         <v>7.3168287060238557E-3</v>
       </c>
       <c r="E8" s="65">
@@ -4970,7 +4973,7 @@
         <f t="shared" si="0"/>
         <v>0.97599999999999998</v>
       </c>
-      <c r="D9" s="31">
+      <c r="D9" s="67">
         <v>8.2126553524233883E-3</v>
       </c>
       <c r="E9" s="65">
@@ -4988,7 +4991,7 @@
         <f t="shared" si="0"/>
         <v>0.97099999999999997</v>
       </c>
-      <c r="D10" s="31">
+      <c r="D10" s="67">
         <v>6.8021830261804951E-3</v>
       </c>
       <c r="E10" s="65">
@@ -5006,7 +5009,7 @@
         <f t="shared" si="0"/>
         <v>0.96199999999999997</v>
       </c>
-      <c r="D11" s="31">
+      <c r="D11" s="67">
         <v>1.0522700306001369E-2</v>
       </c>
       <c r="E11" s="65">
@@ -5024,7 +5027,7 @@
         <f t="shared" si="0"/>
         <v>0.94799999999999995</v>
       </c>
-      <c r="D12" s="31">
+      <c r="D12" s="67">
         <v>1.211535929063693E-2</v>
       </c>
       <c r="E12" s="65">
@@ -5036,17 +5039,17 @@
         <v>2021</v>
       </c>
       <c r="B13" s="31">
-        <v>3.5999999999999997E-2</v>
+        <v>3.5000000000000003E-2</v>
       </c>
       <c r="C13" s="31">
         <f t="shared" si="0"/>
-        <v>0.96399999999999997</v>
-      </c>
-      <c r="D13" s="31">
+        <v>0.96499999999999997</v>
+      </c>
+      <c r="D13" s="67">
         <v>1.252696200431392E-2</v>
       </c>
       <c r="E13" s="65">
-        <v>0.1588950276243094</v>
+        <v>0.158</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Atualização com correções referentes aos dados de 17/12/2021.
</commit_message>
<xml_diff>
--- a/dados/relatorio_historico.xlsx
+++ b/dados/relatorio_historico.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\arian\Desktop\R_STF\Relatorio_R\Git\Code-Relatorio\dados\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA470D17-A01F-4F65-BB09-DE11D091C803}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88B14F82-D944-48F7-AC9E-A5400FB8FC07}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13490" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="5" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11160" firstSheet="5" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="acervo" sheetId="1" r:id="rId1"/>
@@ -4540,8 +4540,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{81CF680A-4DE0-4B0B-AF6A-8D59BB1A8E7B}">
   <dimension ref="A1:H22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="L20" sqref="L20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4783,7 +4783,7 @@
         <v>2020</v>
       </c>
       <c r="C20" s="23">
-        <v>51</v>
+        <v>5828</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
@@ -4794,7 +4794,7 @@
         <v>2020</v>
       </c>
       <c r="C21" s="23">
-        <v>5827</v>
+        <v>51</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
@@ -4809,7 +4809,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B7353AB-3A1D-4F1C-8F3A-DB45EED24601}">
   <dimension ref="A1:E13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K12" sqref="K12"/>
     </sheetView>
   </sheetViews>

</xml_diff>